<commit_message>
30/1 gearing for Z
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-Baby BOM.xlsx
+++ b/Document Library/Bill Of Materials/V-Baby BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Document Library\GitHub\V-Baby CoreXY\Document Library\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1706" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8C6639D8-D77E-4D0F-8FC7-8D12DF099F8D}"/>
+  <xr:revisionPtr revIDLastSave="1708" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{532A1811-B5C6-43E2-9F2E-8802057F72CA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="212">
   <si>
     <t>Exstrusions</t>
   </si>
@@ -354,9 +352,6 @@
     <t>GT2 20T Thoothed Idler</t>
   </si>
   <si>
-    <t>7Pcs 7mm With T</t>
-  </si>
-  <si>
     <t>Belt Idler Smooth</t>
   </si>
   <si>
@@ -667,6 +662,12 @@
   </si>
   <si>
     <t>1/30 Worm Stepper</t>
+  </si>
+  <si>
+    <t>8Pcs 7mm With T</t>
+  </si>
+  <si>
+    <t>Choose the 30/1 gear</t>
   </si>
 </sst>
 </file>
@@ -2022,11 +2023,11 @@
         <v>4</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G1" s="50"/>
       <c r="H1" s="64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I1" s="63"/>
       <c r="J1" s="65" t="s">
@@ -2040,7 +2041,7 @@
       <c r="D2" s="19"/>
       <c r="E2" s="23"/>
       <c r="F2" s="130" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="58"/>
@@ -2218,7 +2219,7 @@
         <v>27</v>
       </c>
       <c r="I10" s="68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J10" s="66">
         <v>27</v>
@@ -2260,7 +2261,7 @@
         <v>31</v>
       </c>
       <c r="I12" s="68" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J12" s="66">
         <v>15</v>
@@ -2298,7 +2299,7 @@
         <v>35</v>
       </c>
       <c r="I14" s="68" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J14" s="66">
         <v>12</v>
@@ -2400,7 +2401,7 @@
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
       <c r="F21" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G21" s="48"/>
       <c r="H21" s="29" t="s">
@@ -2414,7 +2415,7 @@
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -2466,7 +2467,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="105" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="106"/>
       <c r="C1" s="107"/>
@@ -2486,30 +2487,30 @@
     </row>
     <row r="3" spans="1:7" s="104" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="111" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3" s="112"/>
       <c r="C3" s="126" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D3" s="114" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="112"/>
       <c r="F3" s="114" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G3" s="115"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="8">
         <v>310</v>
       </c>
       <c r="C4" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="8">
         <f>B4+50</f>
@@ -2524,38 +2525,38 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="109" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" s="8">
         <v>350</v>
       </c>
       <c r="C5" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="8">
         <f>B5+50</f>
         <v>400</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F5" s="8">
         <f>B5+100</f>
         <v>450</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="109" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" s="8">
         <v>340</v>
       </c>
       <c r="C6" s="127" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" s="8">
         <f>B6+50</f>
@@ -2576,7 +2577,7 @@
         <v>290</v>
       </c>
       <c r="C7" s="127" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" ref="D7:D9" si="0">B7+50</f>
@@ -2597,7 +2598,7 @@
         <v>350</v>
       </c>
       <c r="C8" s="127" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
@@ -2618,7 +2619,7 @@
         <v>295</v>
       </c>
       <c r="C9" s="127" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
@@ -2642,7 +2643,7 @@
     </row>
     <row r="11" spans="1:7" s="104" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="111" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B11" s="112"/>
       <c r="C11" s="113"/>
@@ -2653,7 +2654,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="109" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="110"/>
@@ -2664,14 +2665,14 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="116" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="117"/>
       <c r="C13" s="118" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E13" s="119"/>
       <c r="F13" s="8"/>
@@ -2679,62 +2680,62 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="117">
         <v>200</v>
       </c>
       <c r="C14" s="118" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D14" s="119">
         <f>B14+110</f>
         <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="109" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B15" s="117">
         <v>200</v>
       </c>
       <c r="C15" s="118" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D15" s="119">
         <f>B15+150</f>
         <v>350</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G15" s="13"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="109" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16" s="117">
         <v>200</v>
       </c>
       <c r="C16" s="118" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D16" s="119">
         <f>B16+140</f>
         <v>340</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="13"/>
@@ -2750,7 +2751,7 @@
         <v>290</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="13"/>
@@ -2766,7 +2767,7 @@
         <v>350</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="13"/>
@@ -2782,7 +2783,7 @@
         <v>295</v>
       </c>
       <c r="E19" s="128" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F19" s="124"/>
       <c r="G19" s="125"/>
@@ -2798,17 +2799,17 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2827,7 +2828,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2848,28 +2849,28 @@
   <sheetData>
     <row r="1" spans="1:12" s="75" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C1" s="78" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="D1" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="E1" s="92" t="s">
         <v>177</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="F1" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="76" t="s">
+      <c r="G1" s="85" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="H1" s="85" t="s">
         <v>180</v>
-      </c>
-      <c r="H1" s="85" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2948,7 +2949,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E5" s="84">
         <v>12</v>
@@ -2968,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="84">
         <v>11</v>
@@ -3312,7 +3313,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="129" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="E23" s="33">
         <v>25</v>
@@ -3323,16 +3324,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="C24" s="9">
         <v>6</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E24" s="35">
         <v>22</v>
@@ -3343,16 +3344,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="C25" s="9">
         <v>3</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" s="84">
         <v>30</v>
@@ -3363,43 +3364,45 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E26" s="84">
         <v>37</v>
       </c>
       <c r="F26" s="52"/>
-      <c r="G26" s="57"/>
+      <c r="G26" s="57" t="s">
+        <v>211</v>
+      </c>
       <c r="H26" s="84"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E27" s="84">
         <v>16</v>
       </c>
       <c r="F27" s="52"/>
       <c r="G27" s="93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H27" s="94">
         <v>30</v>
@@ -3407,7 +3410,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -3488,7 +3491,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="97" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -3502,10 +3505,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="C2" s="32">
         <v>2</v>
@@ -3516,10 +3519,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="32">
         <v>4</v>
@@ -3530,10 +3533,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="C4" s="32">
         <v>4</v>
@@ -3544,10 +3547,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="32">
         <v>2</v>
@@ -3558,10 +3561,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="C6" s="32">
         <v>2</v>
@@ -3572,10 +3575,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="32">
         <v>11</v>
@@ -3586,10 +3589,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="C8" s="32">
         <v>15</v>
@@ -3600,10 +3603,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="32">
         <v>6</v>
@@ -3614,10 +3617,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="32">
         <v>9</v>
@@ -3628,10 +3631,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="32">
         <v>5</v>
@@ -3642,10 +3645,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="32">
         <v>8</v>
@@ -3656,10 +3659,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="C13" s="32">
         <v>2</v>
@@ -3670,10 +3673,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="C14" s="32">
         <v>5</v>
@@ -3684,10 +3687,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="32">
         <v>5</v>
@@ -3698,10 +3701,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="32">
         <v>13</v>
@@ -3712,10 +3715,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17" s="32">
         <v>6</v>
@@ -3726,10 +3729,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="32">
         <v>2</v>
@@ -3740,10 +3743,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C19" s="32">
         <v>1</v>
@@ -3754,10 +3757,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" s="32">
         <v>3</v>
@@ -3768,10 +3771,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C21" s="32">
         <v>1</v>
@@ -3782,10 +3785,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="32">
         <v>1</v>
@@ -3796,10 +3799,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="32">
         <v>28</v>
@@ -3810,10 +3813,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" s="32">
         <v>6</v>
@@ -3824,10 +3827,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>148</v>
       </c>
       <c r="C25" s="32">
         <v>50</v>
@@ -3838,10 +3841,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="C26" s="32">
         <v>63</v>
@@ -3852,10 +3855,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="C27" s="32">
         <v>143</v>
@@ -3866,10 +3869,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C28" s="32">
         <v>200</v>
@@ -3880,10 +3883,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" s="32">
         <v>142</v>
@@ -3894,10 +3897,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="32">
         <v>8</v>
@@ -3908,10 +3911,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="32">
         <v>1</v>
@@ -3922,10 +3925,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C32" s="32">
         <v>2</v>
@@ -3936,10 +3939,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" s="32">
         <v>2</v>
@@ -3950,10 +3953,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C34" s="32">
         <v>18</v>
@@ -3964,10 +3967,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C35" s="32">
         <v>8</v>
@@ -3978,10 +3981,10 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C36" s="32">
         <v>4</v>
@@ -3992,7 +3995,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B37" s="71"/>
       <c r="C37" s="100">
@@ -4006,7 +4009,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
@@ -4016,7 +4019,7 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>

</xml_diff>

<commit_message>
duet wifi added to list
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-Baby BOM.xlsx
+++ b/Document Library/Bill Of Materials/V-Baby BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Document Library\GitHub\V-Baby CoreXY\Document Library\Bill Of Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-Baby CoreXY/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1764" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1CF00118-D684-4048-8660-5E6F97288109}"/>
+  <xr:revisionPtr revIDLastSave="1844" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{557D397D-6E27-4DD9-8C58-9C76D84B3D6B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="212">
   <si>
     <t>Exstrusions</t>
   </si>
@@ -171,24 +171,6 @@
     <t>Controller Board</t>
   </si>
   <si>
-    <t>SKR 1.3 32Bit Controller</t>
-  </si>
-  <si>
-    <t>LCD Controller</t>
-  </si>
-  <si>
-    <t>Bique TFT24</t>
-  </si>
-  <si>
-    <t>TFT24 KIT</t>
-  </si>
-  <si>
-    <t>XY Stepper Drivers</t>
-  </si>
-  <si>
-    <t>TMC 2209 Stepper Drivers</t>
-  </si>
-  <si>
     <t>Layer Fan</t>
   </si>
   <si>
@@ -648,18 +630,9 @@
     <t>5x6x1 mm Precision Shim</t>
   </si>
   <si>
-    <t>NB! Choose the 30/1 gear</t>
-  </si>
-  <si>
-    <t>clever3d High End Option</t>
-  </si>
-  <si>
     <t>Keenovo Option</t>
   </si>
   <si>
-    <t>NB! 200 pcs option is same price</t>
-  </si>
-  <si>
     <t>(4x20) 6x5x1 Option Shim</t>
   </si>
   <si>
@@ -669,16 +642,34 @@
     <t>TMC2209 UART x4</t>
   </si>
   <si>
-    <t>TMC2208 UART x4</t>
-  </si>
-  <si>
     <t>SKR 1.4/1.4 Turbo</t>
   </si>
   <si>
-    <t>Board Only</t>
-  </si>
-  <si>
     <t>Heatbed Build Plate</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>200 pcs is same price</t>
+  </si>
+  <si>
+    <t>Choose the 30/1 gear</t>
+  </si>
+  <si>
+    <t>MKS DUET WIFI</t>
+  </si>
+  <si>
+    <t>Duet WIFI Clone w/TMC2660</t>
+  </si>
+  <si>
+    <t>LCD TFT24 KIT</t>
+  </si>
+  <si>
+    <t>V-Baby CoreXY Part List</t>
+  </si>
+  <si>
+    <t>Roy Berntsen</t>
   </si>
 </sst>
 </file>
@@ -688,7 +679,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -777,6 +768,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Freestyle Script"/>
+      <family val="4"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1248,7 +1245,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1420,6 +1417,27 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
@@ -1429,7 +1447,10 @@
     <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1650,17 +1671,73 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723901</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBC55779-0585-41A3-9122-B8EACACCF42B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="1"/>
+          <a:ext cx="723900" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1070DF90-74AC-4245-AA46-2FAD63F74767}" name="Table1" displayName="Table1" ref="A1:G27" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A1:G27" xr:uid="{F74387CC-3A2A-4CC8-A8F2-631B4360BF85}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AB8C8187-911D-4248-8608-1F70796FF7C8}" name="Column1" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1070DF90-74AC-4245-AA46-2FAD63F74767}" name="Table1" displayName="Table1" ref="A1:H30" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:H30" xr:uid="{F74387CC-3A2A-4CC8-A8F2-631B4360BF85}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{AB8C8187-911D-4248-8608-1F70796FF7C8}" name="Column1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{129F7AE4-0D03-4AA3-A2BF-5181AA27AF31}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{34C25536-CCA4-454C-9FCE-0168DD2CC6CC}" name="Column3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{2ABF818D-0A23-4468-A061-EB5B1AC04237}" name="Column4" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{3DD38B84-FE10-46EA-8CEE-8542F56DCDD7}" name="Column5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{E4DF9CF3-4A3D-433E-9BD0-F94DDCA192BB}" name="Column8" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{4866A326-BBBA-4B58-BFBD-4D095130E124}" name="Column9" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{34C25536-CCA4-454C-9FCE-0168DD2CC6CC}" name="Column3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{2ABF818D-0A23-4468-A061-EB5B1AC04237}" name="Column4" dataDxfId="4" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{3DD38B84-FE10-46EA-8CEE-8542F56DCDD7}" name="Column5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{E4DF9CF3-4A3D-433E-9BD0-F94DDCA192BB}" name="Column8" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{4866A326-BBBA-4B58-BFBD-4D095130E124}" name="Column9" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{BCC2F41B-A8C5-4565-9E8A-D5EEC7EF8FC3}" name="Column10" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2020,11 +2097,11 @@
         <v>4</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G1" s="50"/>
       <c r="H1" s="63" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I1" s="62"/>
       <c r="J1" s="64" t="s">
@@ -2038,7 +2115,7 @@
       <c r="D2" s="19"/>
       <c r="E2" s="23"/>
       <c r="F2" s="127" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="57"/>
@@ -2216,7 +2293,7 @@
         <v>27</v>
       </c>
       <c r="I10" s="67" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J10" s="65">
         <v>27</v>
@@ -2258,7 +2335,7 @@
         <v>31</v>
       </c>
       <c r="I12" s="67" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J12" s="65">
         <v>15</v>
@@ -2296,7 +2373,7 @@
         <v>35</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J14" s="65">
         <v>12</v>
@@ -2356,8 +2433,8 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="37">
-        <f>'Component Part List'!$E$28</f>
-        <v>365.5</v>
+        <f>'Component Part List'!$E$31</f>
+        <v>366.5</v>
       </c>
       <c r="G19" s="48"/>
       <c r="H19" s="29" t="s">
@@ -2365,8 +2442,8 @@
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="37">
-        <f>'Component Part List'!$E$28</f>
-        <v>365.5</v>
+        <f>'Component Part List'!$E$31</f>
+        <v>366.5</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2398,7 +2475,7 @@
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
       <c r="F21" s="46" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G21" s="48"/>
       <c r="H21" s="29" t="s">
@@ -2412,7 +2489,7 @@
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="44" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -2420,7 +2497,7 @@
       <c r="E22" s="45"/>
       <c r="F22" s="41">
         <f>SUM(F18:F21)</f>
-        <v>679.5</v>
+        <v>680.5</v>
       </c>
       <c r="G22" s="48"/>
       <c r="H22" s="59" t="s">
@@ -2429,7 +2506,7 @@
       <c r="I22" s="60"/>
       <c r="J22" s="61">
         <f>SUM(J18:J21)</f>
-        <v>550.1</v>
+        <v>551.1</v>
       </c>
     </row>
   </sheetData>
@@ -2464,7 +2541,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="102" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B1" s="103"/>
       <c r="C1" s="104"/>
@@ -2484,30 +2561,30 @@
     </row>
     <row r="3" spans="1:7" s="101" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B3" s="109"/>
       <c r="C3" s="123" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D3" s="111" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E3" s="109"/>
       <c r="F3" s="111" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G3" s="112"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="106" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B4" s="8">
         <v>310</v>
       </c>
       <c r="C4" s="124" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D4" s="8">
         <f>B4+50</f>
@@ -2522,38 +2599,38 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="106" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B5" s="8">
         <v>350</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D5" s="8">
         <f>B5+50</f>
         <v>400</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F5" s="8">
         <f>B5+100</f>
         <v>450</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="106" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B6" s="8">
         <v>340</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D6" s="8">
         <f>B6+50</f>
@@ -2574,7 +2651,7 @@
         <v>290</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" ref="D7:D9" si="0">B7+50</f>
@@ -2595,7 +2672,7 @@
         <v>350</v>
       </c>
       <c r="C8" s="124" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
@@ -2616,7 +2693,7 @@
         <v>295</v>
       </c>
       <c r="C9" s="124" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
@@ -2640,7 +2717,7 @@
     </row>
     <row r="11" spans="1:7" s="101" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="108" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B11" s="109"/>
       <c r="C11" s="110"/>
@@ -2651,7 +2728,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="106" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="107"/>
@@ -2662,14 +2739,14 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="113" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B13" s="114"/>
       <c r="C13" s="115" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D13" s="116" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E13" s="116"/>
       <c r="F13" s="8"/>
@@ -2677,62 +2754,62 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="106" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B14" s="114">
         <v>200</v>
       </c>
       <c r="C14" s="115" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D14" s="116">
         <f>B14+110</f>
         <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="106" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B15" s="114">
         <v>200</v>
       </c>
       <c r="C15" s="115" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D15" s="116">
         <f>B15+150</f>
         <v>350</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G15" s="13"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="106" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B16" s="114">
         <v>200</v>
       </c>
       <c r="C16" s="115" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D16" s="116">
         <f>B16+140</f>
         <v>340</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="13"/>
@@ -2748,7 +2825,7 @@
         <v>290</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="13"/>
@@ -2764,7 +2841,7 @@
         <v>350</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="13"/>
@@ -2780,7 +2857,7 @@
         <v>295</v>
       </c>
       <c r="E19" s="125" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F19" s="121"/>
       <c r="G19" s="122"/>
@@ -2796,17 +2873,17 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2825,7 +2902,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2838,609 +2915,659 @@
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="73" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="73" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="89" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="74" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" s="75" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E1" s="89" t="s">
-        <v>170</v>
-      </c>
-      <c r="F1" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="G1" s="82" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="H1" s="82" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="129"/>
+      <c r="B2" s="129" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="130"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="134"/>
+    </row>
+    <row r="3" spans="1:9" s="73" customFormat="1" ht="27.75" x14ac:dyDescent="0.5">
+      <c r="A3" s="129"/>
+      <c r="B3" s="135" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="130"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="134"/>
+    </row>
+    <row r="4" spans="1:9" s="73" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="129"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="134"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B5" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C5" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D5" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E5" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F5" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="92" t="s">
+      <c r="G5" s="92" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="H5" s="79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="56" t="s">
+        <v>202</v>
+      </c>
+      <c r="G6" s="81">
+        <v>25</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="E3" s="81">
-        <v>20</v>
-      </c>
-      <c r="F3" s="56" t="s">
-        <v>212</v>
-      </c>
-      <c r="G3" s="81">
-        <v>25</v>
-      </c>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="81">
-        <v>15</v>
-      </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="81"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="9">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" s="81">
-        <v>24</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="G5" s="81">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="9">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="81">
-        <v>10</v>
-      </c>
-      <c r="F6" s="56"/>
-      <c r="G6" s="81"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>54</v>
-      </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>208</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>56</v>
+      <c r="D7" s="56" t="s">
+        <v>207</v>
       </c>
       <c r="E7" s="81">
+        <v>60</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G7" s="81">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G8" s="81">
+        <v>24</v>
+      </c>
+      <c r="H8" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="9">
         <v>2</v>
       </c>
-      <c r="F7" s="56"/>
-      <c r="G7" s="81"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="81">
-        <v>3</v>
-      </c>
-      <c r="F8" s="84"/>
-      <c r="G8" s="81"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="9">
-        <v>3</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E9" s="81">
-        <v>4</v>
-      </c>
-      <c r="F9" s="84"/>
+        <v>10</v>
+      </c>
+      <c r="F9" s="56"/>
       <c r="G9" s="81"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>64</v>
+        <v>48</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E10" s="81">
-        <v>14</v>
-      </c>
-      <c r="F10" s="85"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="56"/>
       <c r="G10" s="81"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C11" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E11" s="81">
-        <v>27</v>
-      </c>
-      <c r="F11" s="86" t="s">
-        <v>206</v>
-      </c>
-      <c r="G11" s="81">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F11" s="84"/>
+      <c r="G11" s="81"/>
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C12" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="E12" s="81">
-        <v>3.5</v>
-      </c>
-      <c r="F12" s="86"/>
+        <v>4</v>
+      </c>
+      <c r="F12" s="84"/>
       <c r="G12" s="81"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="C13" s="9">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E13" s="81">
-        <v>2</v>
-      </c>
-      <c r="F13" s="86"/>
+        <v>14</v>
+      </c>
+      <c r="F13" s="85"/>
       <c r="G13" s="81"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E14" s="81">
-        <v>17</v>
-      </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="81"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="F14" s="86" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="81">
+        <v>40</v>
+      </c>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E15" s="81">
-        <v>20</v>
-      </c>
-      <c r="F15" s="56"/>
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="86"/>
       <c r="G15" s="81"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E16" s="81">
-        <v>2.5</v>
-      </c>
-      <c r="F16" s="56"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="86"/>
       <c r="G16" s="81"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E17" s="81">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F17" s="56"/>
       <c r="G17" s="81"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E18" s="81">
-        <v>8.5</v>
+        <v>20</v>
       </c>
       <c r="F18" s="56"/>
       <c r="G18" s="81"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>92</v>
+        <v>76</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E19" s="81">
-        <v>14</v>
+        <v>2.5</v>
       </c>
       <c r="F19" s="56"/>
       <c r="G19" s="81"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C20" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E20" s="81">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F20" s="56"/>
       <c r="G20" s="81"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C21" s="9">
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E21" s="81">
-        <v>6</v>
+        <v>8.5</v>
       </c>
       <c r="F21" s="56"/>
       <c r="G21" s="81"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="81">
+        <v>14</v>
+      </c>
+      <c r="F22" s="56"/>
+      <c r="G22" s="81"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="9">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="81">
+        <v>8</v>
+      </c>
+      <c r="F23" s="56"/>
+      <c r="G23" s="81"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="81">
+        <v>6</v>
+      </c>
+      <c r="F24" s="56"/>
+      <c r="G24" s="81"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="9">
+        <v>7</v>
+      </c>
+      <c r="D25" s="126" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" s="33">
+        <v>25</v>
+      </c>
+      <c r="F25" s="87"/>
+      <c r="G25" s="33"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="9">
+        <v>6</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="35">
+        <v>22</v>
+      </c>
+      <c r="F26" s="88"/>
+      <c r="G26" s="35"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="9">
+        <v>70</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E27" s="35">
+        <v>15</v>
+      </c>
+      <c r="F27" s="56" t="s">
+        <v>205</v>
+      </c>
+      <c r="G27" s="35"/>
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C28" s="9">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="9">
-        <v>7</v>
-      </c>
-      <c r="D22" s="126" t="s">
-        <v>200</v>
-      </c>
-      <c r="E22" s="33">
-        <v>25</v>
-      </c>
-      <c r="F22" s="87"/>
-      <c r="G22" s="33"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="E28" s="81">
+        <v>30</v>
+      </c>
+      <c r="F28" s="56"/>
+      <c r="G28" s="81"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="9">
-        <v>6</v>
-      </c>
-      <c r="D23" s="34" t="s">
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" s="81">
+        <v>37</v>
+      </c>
+      <c r="F29" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="G29" s="81"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="35">
-        <v>22</v>
-      </c>
-      <c r="F23" s="88"/>
-      <c r="G23" s="35"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="C24" s="9">
-        <v>70</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E24" s="35">
-        <v>15</v>
-      </c>
-      <c r="F24" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="G24" s="35"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="E30" s="81">
+        <v>16</v>
+      </c>
+      <c r="F30" s="90"/>
+      <c r="G30" s="91"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="9">
-        <v>3</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E25" s="81">
-        <v>30</v>
-      </c>
-      <c r="F25" s="56"/>
-      <c r="G25" s="81"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="9">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E26" s="81">
-        <v>37</v>
-      </c>
-      <c r="F26" s="56" t="s">
-        <v>204</v>
-      </c>
-      <c r="G26" s="81"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="9">
-        <v>1</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="81">
-        <v>16</v>
-      </c>
-      <c r="F27" s="90" t="s">
-        <v>205</v>
-      </c>
-      <c r="G27" s="91">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="72">
-        <f>SUM(E2:E27)</f>
-        <v>365.5</v>
-      </c>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="72">
+        <f>SUM(E2:E30)</f>
+        <v>366.5</v>
+      </c>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D27" r:id="rId1" display="5mm 220x220" xr:uid="{A5B2720F-8C3E-478A-BE06-E55BE0B574B4}"/>
-    <hyperlink ref="D11" r:id="rId2" xr:uid="{3773511A-F3AF-4897-B5BB-16FB39A0B508}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{AFC120EB-E75F-4BB8-BC6D-4AA9408DD14D}"/>
-    <hyperlink ref="D17" r:id="rId4" display="Link" xr:uid="{401DDADA-DB79-4416-96CF-3B1D6329769B}"/>
-    <hyperlink ref="D6" r:id="rId5" display="24V Dual Ball" xr:uid="{98BCAD8D-1DD9-49E5-B60D-FB8A39108E71}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{968A8156-5055-4A5F-97A2-06DF8EA0EB3D}"/>
-    <hyperlink ref="D19" r:id="rId7" display="5 Meter Gates LL" xr:uid="{9F0DE403-B0EC-4933-928F-2806FBCF603A}"/>
-    <hyperlink ref="D18" r:id="rId8" display="Link" xr:uid="{45531F32-6B6C-44D5-9B2A-FB1F259BC9F9}"/>
-    <hyperlink ref="F11" r:id="rId9" display="Keenovo" xr:uid="{C2A02BBB-B317-4856-A562-A30BE2CA0A6C}"/>
-    <hyperlink ref="D21" r:id="rId10" display="8 Bore" xr:uid="{4C50ADBB-FC9C-42E4-8421-5A0C1600DD46}"/>
-    <hyperlink ref="D20" r:id="rId11" display="5 BORE" xr:uid="{43C03DCA-7867-4C9F-B1D0-8588267A1C82}"/>
-    <hyperlink ref="D12" r:id="rId12" xr:uid="{A901DFE1-486C-4AC2-8672-C18618945E04}"/>
-    <hyperlink ref="D13" r:id="rId13" xr:uid="{BA467D2F-0948-4A82-B49C-B8DCBA7936A0}"/>
-    <hyperlink ref="D25" r:id="rId14" display="Link" xr:uid="{49178A12-AF45-4969-AC8E-49BA3EBADDA9}"/>
-    <hyperlink ref="D3" r:id="rId15" display="Board" xr:uid="{EC545E70-D1FC-4E65-A1EE-4669C3053F17}"/>
-    <hyperlink ref="D5" r:id="rId16" display="TMC2209x4" xr:uid="{66F0B115-3A28-4ECD-9CAD-3D7BD72D9C3F}"/>
-    <hyperlink ref="D15" r:id="rId17" xr:uid="{9689F2B7-24E0-4CC5-A39F-53D7E0370FC8}"/>
-    <hyperlink ref="D14" r:id="rId18" xr:uid="{537A3F3C-7C92-42A9-B8B2-F37129F7787F}"/>
-    <hyperlink ref="D4" r:id="rId19" display="Mini 12864" xr:uid="{56BAC9A8-6A57-4E69-944B-AE64A70C2A1E}"/>
-    <hyperlink ref="D16" r:id="rId20" xr:uid="{82909F8B-3A14-4248-8CB2-384756C6E8BE}"/>
-    <hyperlink ref="D26" r:id="rId21" xr:uid="{0D6A5659-9181-49D0-A7D8-101F63076C8A}"/>
-    <hyperlink ref="F27" r:id="rId22" display="CLEVER3D" xr:uid="{7B1D2EFC-9E0A-4BD0-B66C-2C091262564C}"/>
-    <hyperlink ref="D9" r:id="rId23" xr:uid="{4AEFCE09-28B7-4C24-82DE-ADAB9CAA43E1}"/>
-    <hyperlink ref="D10" r:id="rId24" xr:uid="{0ED2334F-09CF-437E-82F8-E81D86F288DC}"/>
-    <hyperlink ref="D22" r:id="rId25" xr:uid="{87CB364F-700B-4E81-BC67-3C859C1B7934}"/>
-    <hyperlink ref="D23" r:id="rId26" display="5X High End" xr:uid="{D4CB98E8-7A2B-495D-9E37-8208D21A6270}"/>
-    <hyperlink ref="D24" r:id="rId27" display="6x5x1 Option Shim" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
-    <hyperlink ref="F24" r:id="rId28" xr:uid="{D98A7A59-4D4C-4589-8C00-1DCF83FFF3E6}"/>
-    <hyperlink ref="F5" r:id="rId29" display="TMC2209x4" xr:uid="{5A565AD2-589F-454F-8FE2-3DC1AA6ECAC6}"/>
-    <hyperlink ref="F3" r:id="rId30" xr:uid="{5B14FBB6-ADAD-4948-95D7-FBD8C9BC5BB5}"/>
+    <hyperlink ref="D30" r:id="rId1" display="5mm 220x220" xr:uid="{A5B2720F-8C3E-478A-BE06-E55BE0B574B4}"/>
+    <hyperlink ref="D14" r:id="rId2" xr:uid="{3773511A-F3AF-4897-B5BB-16FB39A0B508}"/>
+    <hyperlink ref="D11" r:id="rId3" xr:uid="{AFC120EB-E75F-4BB8-BC6D-4AA9408DD14D}"/>
+    <hyperlink ref="D20" r:id="rId4" display="Link" xr:uid="{401DDADA-DB79-4416-96CF-3B1D6329769B}"/>
+    <hyperlink ref="D9" r:id="rId5" display="24V Dual Ball" xr:uid="{98BCAD8D-1DD9-49E5-B60D-FB8A39108E71}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{968A8156-5055-4A5F-97A2-06DF8EA0EB3D}"/>
+    <hyperlink ref="D22" r:id="rId7" display="5 Meter Gates LL" xr:uid="{9F0DE403-B0EC-4933-928F-2806FBCF603A}"/>
+    <hyperlink ref="D21" r:id="rId8" display="Link" xr:uid="{45531F32-6B6C-44D5-9B2A-FB1F259BC9F9}"/>
+    <hyperlink ref="F14" r:id="rId9" display="Keenovo" xr:uid="{C2A02BBB-B317-4856-A562-A30BE2CA0A6C}"/>
+    <hyperlink ref="D24" r:id="rId10" display="8 Bore" xr:uid="{4C50ADBB-FC9C-42E4-8421-5A0C1600DD46}"/>
+    <hyperlink ref="D23" r:id="rId11" display="5 BORE" xr:uid="{43C03DCA-7867-4C9F-B1D0-8588267A1C82}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{A901DFE1-486C-4AC2-8672-C18618945E04}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{BA467D2F-0948-4A82-B49C-B8DCBA7936A0}"/>
+    <hyperlink ref="D28" r:id="rId14" display="Link" xr:uid="{49178A12-AF45-4969-AC8E-49BA3EBADDA9}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{9689F2B7-24E0-4CC5-A39F-53D7E0370FC8}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{537A3F3C-7C92-42A9-B8B2-F37129F7787F}"/>
+    <hyperlink ref="D19" r:id="rId17" xr:uid="{82909F8B-3A14-4248-8CB2-384756C6E8BE}"/>
+    <hyperlink ref="D29" r:id="rId18" xr:uid="{0D6A5659-9181-49D0-A7D8-101F63076C8A}"/>
+    <hyperlink ref="D12" r:id="rId19" xr:uid="{4AEFCE09-28B7-4C24-82DE-ADAB9CAA43E1}"/>
+    <hyperlink ref="D13" r:id="rId20" xr:uid="{0ED2334F-09CF-437E-82F8-E81D86F288DC}"/>
+    <hyperlink ref="D25" r:id="rId21" xr:uid="{87CB364F-700B-4E81-BC67-3C859C1B7934}"/>
+    <hyperlink ref="D26" r:id="rId22" display="5X High End" xr:uid="{D4CB98E8-7A2B-495D-9E37-8208D21A6270}"/>
+    <hyperlink ref="D27" r:id="rId23" display="6x5x1 Option Shim" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
+    <hyperlink ref="F27" r:id="rId24" display="NB! 200 pcs option is same price" xr:uid="{D98A7A59-4D4C-4589-8C00-1DCF83FFF3E6}"/>
+    <hyperlink ref="F6" r:id="rId25" xr:uid="{5B14FBB6-ADAD-4948-95D7-FBD8C9BC5BB5}"/>
+    <hyperlink ref="D7" r:id="rId26" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
+    <hyperlink ref="F8" r:id="rId27" display="TMC2209x4" xr:uid="{94AC3372-BF50-48D8-845E-F71522DA0595}"/>
+    <hyperlink ref="F7" r:id="rId28" display="Mini 12864" xr:uid="{321ACA62-20AB-45F9-A643-EE2EB664C961}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId29"/>
+  <drawing r:id="rId30"/>
   <tableParts count="1">
-    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3475,7 +3602,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="94" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -3489,10 +3616,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C2" s="32">
         <v>2</v>
@@ -3503,10 +3630,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C3" s="32">
         <v>4</v>
@@ -3517,10 +3644,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C4" s="32">
         <v>4</v>
@@ -3531,10 +3658,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C5" s="32">
         <v>2</v>
@@ -3545,10 +3672,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C6" s="32">
         <v>2</v>
@@ -3559,10 +3686,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C7" s="32">
         <v>11</v>
@@ -3573,10 +3700,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C8" s="32">
         <v>15</v>
@@ -3587,10 +3714,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C9" s="32">
         <v>6</v>
@@ -3601,10 +3728,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C10" s="32">
         <v>9</v>
@@ -3615,10 +3742,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C11" s="32">
         <v>5</v>
@@ -3629,10 +3756,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C12" s="32">
         <v>8</v>
@@ -3643,10 +3770,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C13" s="32">
         <v>2</v>
@@ -3657,10 +3784,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C14" s="32">
         <v>5</v>
@@ -3671,10 +3798,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C15" s="32">
         <v>5</v>
@@ -3685,10 +3812,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C16" s="32">
         <v>13</v>
@@ -3699,10 +3826,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C17" s="32">
         <v>6</v>
@@ -3713,10 +3840,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C18" s="32">
         <v>2</v>
@@ -3727,10 +3854,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C19" s="32">
         <v>1</v>
@@ -3741,10 +3868,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C20" s="32">
         <v>3</v>
@@ -3755,10 +3882,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C21" s="32">
         <v>1</v>
@@ -3769,10 +3896,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C22" s="32">
         <v>1</v>
@@ -3783,10 +3910,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C23" s="32">
         <v>28</v>
@@ -3797,10 +3924,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C24" s="32">
         <v>6</v>
@@ -3811,10 +3938,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C25" s="32">
         <v>50</v>
@@ -3825,10 +3952,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C26" s="32">
         <v>63</v>
@@ -3837,15 +3964,15 @@
         <v>70</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C27" s="32">
         <v>143</v>
@@ -3856,10 +3983,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C28" s="32">
         <v>200</v>
@@ -3870,10 +3997,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C29" s="32">
         <v>142</v>
@@ -3884,10 +4011,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C30" s="32">
         <v>8</v>
@@ -3898,10 +4025,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C31" s="32">
         <v>1</v>
@@ -3912,10 +4039,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C32" s="32">
         <v>2</v>
@@ -3926,10 +4053,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C33" s="32">
         <v>2</v>
@@ -3940,10 +4067,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C34" s="32">
         <v>18</v>
@@ -3954,10 +4081,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C35" s="32">
         <v>8</v>
@@ -3968,10 +4095,10 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C36" s="32">
         <v>4</v>
@@ -3982,7 +4109,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="69" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B37" s="70"/>
       <c r="C37" s="97">
@@ -3996,7 +4123,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
@@ -4006,7 +4133,7 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>

</xml_diff>

<commit_message>
sorting by name in list
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-Baby BOM.xlsx
+++ b/Document Library/Bill Of Materials/V-Baby BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-Baby CoreXY/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1908" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D72271CF-579D-4894-A17A-3CF834891BA1}"/>
+  <xr:revisionPtr revIDLastSave="1955" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FB102730-A57A-4165-89BD-8C428997DB2C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpenBuild Part List" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="222">
   <si>
     <t>Exstrusions</t>
   </si>
@@ -525,9 +525,6 @@
     <t>Column8</t>
   </si>
   <si>
-    <t>Column9</t>
-  </si>
-  <si>
     <t>M3x30 HEX</t>
   </si>
   <si>
@@ -633,9 +630,6 @@
     <t>Heatbed Build Plate</t>
   </si>
   <si>
-    <t>Column10</t>
-  </si>
-  <si>
     <t>200 pcs is same price</t>
   </si>
   <si>
@@ -681,13 +675,31 @@
     <t>Sleeve for Heatbed cables</t>
   </si>
   <si>
-    <t>Nylon Cable Sleeve</t>
-  </si>
-  <si>
     <t>Tube for Hotend Cables</t>
   </si>
   <si>
     <t>10 mm Sleeve</t>
+  </si>
+  <si>
+    <t>Cable Sleeve Nylon</t>
+  </si>
+  <si>
+    <t>SKR Option -&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>--- &gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Controller Option</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
   </si>
 </sst>
 </file>
@@ -871,7 +883,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -909,21 +921,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1104,19 +1101,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -1125,17 +1109,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1187,32 +1160,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1245,6 +1192,43 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1263,56 +1247,48 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1322,27 +1298,26 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="24" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="21" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1355,47 +1330,32 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="28" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="29" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1413,29 +1373,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1451,12 +1404,75 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="26" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
@@ -1702,8 +1718,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>723901</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171452</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1746,17 +1762,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1070DF90-74AC-4245-AA46-2FAD63F74767}" name="Table1" displayName="Table1" ref="A1:H31" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A1:H31" xr:uid="{F74387CC-3A2A-4CC8-A8F2-631B4360BF85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1070DF90-74AC-4245-AA46-2FAD63F74767}" name="Table1" displayName="Table1" ref="A1:H30" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:H30" xr:uid="{F74387CC-3A2A-4CC8-A8F2-631B4360BF85}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H30">
+    <sortCondition ref="A5:A30"/>
+  </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AB8C8187-911D-4248-8608-1F70796FF7C8}" name="Column1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{129F7AE4-0D03-4AA3-A2BF-5181AA27AF31}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{34C25536-CCA4-454C-9FCE-0168DD2CC6CC}" name="Column3" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{2ABF818D-0A23-4468-A061-EB5B1AC04237}" name="Column4" dataDxfId="4" dataCellStyle="Hyperlink"/>
     <tableColumn id="5" xr3:uid="{3DD38B84-FE10-46EA-8CEE-8542F56DCDD7}" name="Column5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{E4DF9CF3-4A3D-433E-9BD0-F94DDCA192BB}" name="Column8" dataDxfId="2" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{4866A326-BBBA-4B58-BFBD-4D095130E124}" name="Column9" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{BCC2F41B-A8C5-4565-9E8A-D5EEC7EF8FC3}" name="Column10" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{E4DF9CF3-4A3D-433E-9BD0-F94DDCA192BB}" name="Column6" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{4866A326-BBBA-4B58-BFBD-4D095130E124}" name="Column7" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{BCC2F41B-A8C5-4565-9E8A-D5EEC7EF8FC3}" name="Column8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2100,430 +2119,430 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="63" t="s">
+      <c r="G1" s="44"/>
+      <c r="H1" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="64" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="58" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="135" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="114" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="65"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>4</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="10">
         <f>D3*310</f>
         <v>1240</v>
       </c>
-      <c r="F3" s="136"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="66"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="60"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="24">
         <v>4</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="23">
         <f>D4*350</f>
         <v>1400</v>
       </c>
-      <c r="F4" s="136"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="65"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>5</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <f>D5*340</f>
         <v>1700</v>
       </c>
-      <c r="F5" s="136"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="66"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="24">
         <v>1</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="23">
         <f>D6*295</f>
         <v>295</v>
       </c>
-      <c r="F6" s="136"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="65"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="66"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="60"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="24">
         <v>1</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="23">
         <f>D8*290</f>
         <v>290</v>
       </c>
-      <c r="F8" s="136"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="65"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <f>D9*350</f>
         <v>700</v>
       </c>
-      <c r="F9" s="136"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="66"/>
-    </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="F9" s="115"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="60"/>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="25">
+      <c r="D10" s="24"/>
+      <c r="E10" s="22">
         <f>SUM(E3:E9)</f>
         <v>5625</v>
       </c>
-      <c r="F10" s="136"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="58" t="s">
+      <c r="F10" s="115"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="67" t="s">
+      <c r="I10" s="61" t="s">
         <v>154</v>
       </c>
-      <c r="J10" s="65">
+      <c r="J10" s="59">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="136"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="29" t="s">
+      <c r="A11" s="48"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="68"/>
-      <c r="J11" s="66">
+      <c r="I11" s="62"/>
+      <c r="J11" s="60">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="24">
         <v>18</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="136"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="58" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="67" t="s">
+      <c r="I12" s="61" t="s">
         <v>155</v>
       </c>
-      <c r="J12" s="65">
+      <c r="J12" s="59">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="136"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="66"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="60"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="24">
         <v>30</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="136"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="58" t="s">
+      <c r="E14" s="21"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="67" t="s">
+      <c r="I14" s="61" t="s">
         <v>156</v>
       </c>
-      <c r="J14" s="65">
+      <c r="J14" s="59">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="28">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="25">
         <v>314</v>
       </c>
-      <c r="G15" s="51"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="28">
+      <c r="G15" s="45"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="25">
         <f>SUM(J2:J14)</f>
         <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G16" s="17"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="36">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="30">
         <f>F15</f>
         <v>314</v>
       </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="39" t="s">
+      <c r="G18" s="42"/>
+      <c r="H18" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="42"/>
-      <c r="J18" s="36">
+      <c r="I18" s="36"/>
+      <c r="J18" s="30">
         <f>J15</f>
         <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="37">
-        <f>'Component Part List'!$E$32</f>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="31">
+        <f>'Component Part List'!$E$31</f>
         <v>394</v>
       </c>
-      <c r="G19" s="48"/>
-      <c r="H19" s="29" t="s">
+      <c r="G19" s="42"/>
+      <c r="H19" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="37">
-        <f>'Component Part List'!$E$32</f>
+      <c r="I19" s="6"/>
+      <c r="J19" s="31">
+        <f>'Component Part List'!$E$31</f>
         <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="38" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="48"/>
-      <c r="H20" s="30" t="s">
+      <c r="G20" s="42"/>
+      <c r="H20" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="27"/>
-      <c r="J20" s="38" t="s">
+      <c r="I20" s="24"/>
+      <c r="J20" s="32" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="46" t="s">
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="G21" s="48"/>
-      <c r="H21" s="29" t="s">
+      <c r="G21" s="42"/>
+      <c r="H21" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="8"/>
-      <c r="J21" s="37">
+      <c r="I21" s="6"/>
+      <c r="J21" s="31">
         <f>Fasteners!D39</f>
         <v>80.600000000000009</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="41">
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="35">
         <f>SUM(F18:F21)</f>
         <v>708</v>
       </c>
-      <c r="G22" s="48"/>
-      <c r="H22" s="59" t="s">
+      <c r="G22" s="42"/>
+      <c r="H22" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="60"/>
-      <c r="J22" s="61">
+      <c r="I22" s="54"/>
+      <c r="J22" s="55">
         <f>SUM(J18:J21)</f>
         <v>578.6</v>
       </c>
@@ -2554,355 +2573,355 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="100" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="82" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="84" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="87"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="88"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" s="83" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="90" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="105"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="106"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:7" s="101" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="108" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="109"/>
-      <c r="C3" s="123" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="111" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="105" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="93" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="91"/>
+      <c r="F3" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="109"/>
-      <c r="F3" s="111" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="112"/>
+      <c r="G3" s="94"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="106" t="s">
-        <v>181</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="A4" s="88" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="6">
         <v>310</v>
       </c>
-      <c r="C4" s="124" t="s">
-        <v>184</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="C4" s="106" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="6">
         <f>B4+50</f>
         <v>360</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6">
         <f>B4+100</f>
         <v>410</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="106" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="A5" s="88" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="6">
         <v>350</v>
       </c>
-      <c r="C5" s="124" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" s="8">
+      <c r="C5" s="106" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="6">
         <f>B5+50</f>
         <v>400</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="6">
         <f>B5+100</f>
         <v>450</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>189</v>
+      <c r="G5" s="10" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
-        <v>183</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="A6" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="6">
         <v>340</v>
       </c>
-      <c r="C6" s="124" t="s">
-        <v>185</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="C6" s="106" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="6">
         <f>B6+50</f>
         <v>390</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
         <f>B6+100</f>
         <v>440</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="14">
         <v>290</v>
       </c>
-      <c r="C7" s="124" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" s="8">
+      <c r="C7" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="6">
         <f t="shared" ref="D7:D9" si="0">B7+50</f>
         <v>340</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
         <f t="shared" ref="F7:F9" si="1">B7+100</f>
         <v>390</v>
       </c>
-      <c r="G7" s="13"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="14">
         <v>350</v>
       </c>
-      <c r="C8" s="124" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="8">
+      <c r="C8" s="106" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
         <f t="shared" si="1"/>
         <v>450</v>
       </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="106" t="s">
+      <c r="A9" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="14">
         <v>295</v>
       </c>
-      <c r="C9" s="124" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" s="8">
+      <c r="C9" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>345</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>395</v>
       </c>
-      <c r="G9" s="13"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="106"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" s="101" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="108" t="s">
+      <c r="A10" s="88"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" s="83" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="90" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="94"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="88" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="95" t="s">
         <v>174</v>
       </c>
-      <c r="B11" s="109"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="112"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="106" t="s">
-        <v>173</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="113" t="s">
+      <c r="B13" s="96"/>
+      <c r="C13" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="98" t="s">
         <v>175</v>
       </c>
-      <c r="B13" s="114"/>
-      <c r="C13" s="115" t="s">
-        <v>177</v>
-      </c>
-      <c r="D13" s="116" t="s">
-        <v>176</v>
-      </c>
-      <c r="E13" s="116"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="13"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="106" t="s">
-        <v>181</v>
-      </c>
-      <c r="B14" s="114">
+      <c r="A14" s="88" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="96">
         <v>200</v>
       </c>
-      <c r="C14" s="115" t="s">
-        <v>168</v>
-      </c>
-      <c r="D14" s="116">
+      <c r="C14" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="98">
         <f>B14+110</f>
         <v>310</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="13"/>
+      <c r="E14" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="106" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15" s="114">
+      <c r="A15" s="88" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="96">
         <v>200</v>
       </c>
-      <c r="C15" s="115" t="s">
-        <v>169</v>
-      </c>
-      <c r="D15" s="116">
+      <c r="C15" s="97" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="98">
         <f>B15+150</f>
         <v>350</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="G15" s="13"/>
+      <c r="E15" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="106" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="114">
+      <c r="A16" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="96">
         <v>200</v>
       </c>
-      <c r="C16" s="115" t="s">
-        <v>170</v>
-      </c>
-      <c r="D16" s="116">
+      <c r="C16" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" s="98">
         <f>B16+140</f>
         <v>340</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="13"/>
+      <c r="E16" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="106" t="s">
+      <c r="A17" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="114"/>
-      <c r="C17" s="115"/>
-      <c r="D17" s="116">
+      <c r="B17" s="96"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="98">
         <f>B14+90</f>
         <v>290</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="13"/>
+      <c r="E17" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="106" t="s">
+      <c r="A18" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="116">
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="98">
         <f>B15+150</f>
         <v>350</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="13"/>
+      <c r="E18" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="117" t="s">
+      <c r="A19" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="118"/>
-      <c r="C19" s="119"/>
-      <c r="D19" s="120">
+      <c r="B19" s="100"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="102">
         <f>B14+95</f>
         <v>295</v>
       </c>
-      <c r="E19" s="125" t="s">
-        <v>186</v>
-      </c>
-      <c r="F19" s="121"/>
-      <c r="G19" s="122"/>
+      <c r="E19" s="107" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19" s="103"/>
+      <c r="G19" s="104"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2921,11 +2940,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2934,693 +2951,691 @@
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="14" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="73" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:9" s="66" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="82" t="s">
-        <v>163</v>
-      </c>
-      <c r="H1" s="82" t="s">
+    </row>
+    <row r="2" spans="1:9" s="66" customFormat="1" ht="27.75" x14ac:dyDescent="0.5">
+      <c r="A2" s="135"/>
+      <c r="B2" s="112" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="136"/>
+      <c r="D2" s="108" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" s="137"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="139"/>
+    </row>
+    <row r="3" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="118"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="124"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="133" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="134" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="119" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="134" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="134" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="119" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="119" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="148" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="141">
+        <v>80</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" s="143">
+        <v>15</v>
+      </c>
+      <c r="F5" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="150"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="111"/>
+    </row>
+    <row r="6" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="120">
+        <v>6</v>
+      </c>
+      <c r="D6" s="123" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="144">
+        <v>22</v>
+      </c>
+      <c r="F6" s="74"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="111"/>
+    </row>
+    <row r="7" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="120">
+        <v>7</v>
+      </c>
+      <c r="D7" s="140" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="145">
+        <v>25</v>
+      </c>
+      <c r="F7" s="73"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="111"/>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="120">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="146">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="50"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="120">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="146">
+        <v>3</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="130" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" s="120">
+        <v>1</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="146">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="50"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="120">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="E11" s="146">
+        <v>8</v>
+      </c>
+      <c r="F11" s="50"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="131"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="127"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="127" t="s">
+      <c r="C12" s="120">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="146">
+        <v>60</v>
+      </c>
+      <c r="F12" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="G12" s="113">
+        <v>15</v>
+      </c>
+      <c r="H12" s="132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="120" t="s">
+        <v>217</v>
+      </c>
+      <c r="D13" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="E13" s="146"/>
+      <c r="F13" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="113">
+        <v>45</v>
+      </c>
+      <c r="H13" s="132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="120">
+        <v>1</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="146">
+        <v>20</v>
+      </c>
+      <c r="F14" s="50"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="E2" s="130"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="132"/>
-    </row>
-    <row r="3" spans="1:9" s="73" customFormat="1" ht="27.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="127"/>
-      <c r="B3" s="133" t="s">
+      <c r="C15" s="120">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="128"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="131"/>
-      <c r="I3" s="132"/>
-    </row>
-    <row r="4" spans="1:9" s="73" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="127"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="132"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
+      <c r="E15" s="146">
+        <v>30</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="113">
+        <v>16</v>
+      </c>
+      <c r="H15" s="131"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="120">
         <v>1</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="D16" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="146">
         <v>2</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="F16" s="50"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="120">
+        <v>2</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="146">
+        <v>10</v>
+      </c>
+      <c r="F17" s="50"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="120">
+        <v>2</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="146">
+        <v>8</v>
+      </c>
+      <c r="F18" s="50"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="120">
+        <v>1</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="146">
+        <v>6</v>
+      </c>
+      <c r="F19" s="50"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="31"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="120">
         <v>3</v>
       </c>
-      <c r="D5" s="80" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" s="93" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="83" t="s">
-        <v>211</v>
-      </c>
-      <c r="G5" s="92" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="79" t="s">
+      <c r="D20" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="146">
+        <v>30</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="31"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="120">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="G6" s="81">
-        <v>45</v>
-      </c>
-      <c r="H6" s="9">
+      <c r="D21" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="146">
+        <v>4</v>
+      </c>
+      <c r="F21" s="71"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="31"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="120">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="D22" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="146">
+        <v>8.5</v>
+      </c>
+      <c r="F22" s="50"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="31"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="120">
         <v>1</v>
       </c>
-      <c r="D7" s="56" t="s">
-        <v>209</v>
-      </c>
-      <c r="E7" s="81">
+      <c r="D23" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="146">
+        <v>20</v>
+      </c>
+      <c r="F23" s="50"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="31"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="120">
+        <v>1</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="146">
+        <v>2</v>
+      </c>
+      <c r="F24" s="72"/>
+      <c r="G24" s="113"/>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="G7" s="81">
-        <v>15</v>
-      </c>
-      <c r="H7" s="9">
+      <c r="C25" s="120">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="81">
-        <v>10</v>
-      </c>
-      <c r="F8" s="56"/>
-      <c r="G8" s="81"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="9">
+      <c r="D25" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="146">
+        <v>30</v>
+      </c>
+      <c r="F25" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="G25" s="113">
+        <v>40</v>
+      </c>
+      <c r="H25" s="131">
         <v>1</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="81">
-        <v>2</v>
-      </c>
-      <c r="F9" s="56"/>
-      <c r="G9" s="81"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="81">
-        <v>3</v>
-      </c>
-      <c r="F10" s="84"/>
-      <c r="G10" s="81"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="9">
-        <v>3</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="81">
-        <v>4</v>
-      </c>
-      <c r="F11" s="84"/>
-      <c r="G11" s="81"/>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="120">
+        <v>1</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="146">
+        <v>3.5</v>
+      </c>
+      <c r="F26" s="72"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="31"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="120" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="146">
+        <v>14</v>
+      </c>
+      <c r="F27" s="50"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="31"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="120">
+        <v>1</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="146">
+        <v>17</v>
+      </c>
+      <c r="F28" s="50"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="31"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="120">
+        <v>1</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E29" s="146">
+        <v>37</v>
+      </c>
+      <c r="F29" s="50"/>
+      <c r="G29" s="113"/>
+      <c r="H29" s="131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B30" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C30" s="142">
         <v>1</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D30" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="81">
+      <c r="E30" s="147">
         <v>14</v>
       </c>
-      <c r="F12" s="85"/>
-      <c r="G12" s="81"/>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="81">
-        <v>30</v>
-      </c>
-      <c r="F13" s="86" t="s">
-        <v>195</v>
-      </c>
-      <c r="G13" s="81">
-        <v>40</v>
-      </c>
-      <c r="H13" s="100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="9">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="81">
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="86"/>
-      <c r="G14" s="81"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="81">
-        <v>2</v>
-      </c>
-      <c r="F15" s="86"/>
-      <c r="G15" s="81"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="9">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="81">
-        <v>17</v>
-      </c>
-      <c r="F16" s="56"/>
-      <c r="G16" s="81"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="9">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="81">
-        <v>20</v>
-      </c>
-      <c r="F17" s="56"/>
-      <c r="G17" s="81"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="9">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="81">
-        <v>2.5</v>
-      </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="81"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="9">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="81">
-        <v>20</v>
-      </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="81"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="9">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="81">
-        <v>8.5</v>
-      </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="81"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="81">
-        <v>14</v>
-      </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="81"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="9">
-        <v>2</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="81">
-        <v>8</v>
-      </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="81"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="9">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="81">
-        <v>6</v>
-      </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="81"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="9">
-        <v>7</v>
-      </c>
-      <c r="D24" s="126" t="s">
-        <v>191</v>
-      </c>
-      <c r="E24" s="33">
-        <v>25</v>
-      </c>
-      <c r="F24" s="87"/>
-      <c r="G24" s="33"/>
-      <c r="H24"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="9">
-        <v>6</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="35">
-        <v>22</v>
-      </c>
-      <c r="F25" s="88"/>
-      <c r="G25" s="35"/>
-      <c r="H25"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C26" s="9">
-        <v>70</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E26" s="35">
-        <v>15</v>
-      </c>
-      <c r="F26" s="56" t="s">
-        <v>200</v>
-      </c>
-      <c r="G26" s="35"/>
-      <c r="H26"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="9">
-        <v>3</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="81">
-        <v>30</v>
-      </c>
-      <c r="F27" s="56"/>
-      <c r="G27" s="81"/>
-      <c r="H27"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="9">
-        <v>1</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E28" s="81">
-        <v>37</v>
-      </c>
-      <c r="F28" s="56"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C29" s="9">
-        <v>1</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E29" s="134">
-        <v>30</v>
-      </c>
-      <c r="F29" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="G29" s="81">
-        <v>16</v>
-      </c>
-      <c r="H29" s="100"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C30" s="9">
-        <v>1</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E30" s="134">
-        <v>8</v>
-      </c>
-      <c r="F30" s="56"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="100"/>
+      <c r="F30" s="151"/>
+      <c r="G30" s="152"/>
+      <c r="H30" s="117"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="B31" t="s">
-        <v>216</v>
-      </c>
-      <c r="C31" s="9">
-        <v>1</v>
-      </c>
-      <c r="D31" s="56" t="s">
-        <v>212</v>
-      </c>
-      <c r="E31" s="81">
-        <v>2.5</v>
-      </c>
-      <c r="F31" s="90"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+      <c r="A31" s="125" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="72">
-        <f>SUM(E6:E31)</f>
+      <c r="B31" s="126"/>
+      <c r="C31" s="126"/>
+      <c r="D31" s="126"/>
+      <c r="E31" s="127">
+        <f>SUM(E5:E30)</f>
         <v>394</v>
       </c>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1" xr:uid="{3773511A-F3AF-4897-B5BB-16FB39A0B508}"/>
-    <hyperlink ref="D10" r:id="rId2" xr:uid="{AFC120EB-E75F-4BB8-BC6D-4AA9408DD14D}"/>
-    <hyperlink ref="D19" r:id="rId3" display="Link" xr:uid="{401DDADA-DB79-4416-96CF-3B1D6329769B}"/>
-    <hyperlink ref="D8" r:id="rId4" display="24V Dual Ball" xr:uid="{98BCAD8D-1DD9-49E5-B60D-FB8A39108E71}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{968A8156-5055-4A5F-97A2-06DF8EA0EB3D}"/>
-    <hyperlink ref="D21" r:id="rId6" display="5 Meter Gates LL" xr:uid="{9F0DE403-B0EC-4933-928F-2806FBCF603A}"/>
-    <hyperlink ref="D20" r:id="rId7" display="Link" xr:uid="{45531F32-6B6C-44D5-9B2A-FB1F259BC9F9}"/>
-    <hyperlink ref="F13" r:id="rId8" display="Keenovo" xr:uid="{C2A02BBB-B317-4856-A562-A30BE2CA0A6C}"/>
-    <hyperlink ref="D23" r:id="rId9" display="8 Bore" xr:uid="{4C50ADBB-FC9C-42E4-8421-5A0C1600DD46}"/>
-    <hyperlink ref="D22" r:id="rId10" display="5 BORE" xr:uid="{43C03DCA-7867-4C9F-B1D0-8588267A1C82}"/>
-    <hyperlink ref="D14" r:id="rId11" xr:uid="{A901DFE1-486C-4AC2-8672-C18618945E04}"/>
-    <hyperlink ref="D15" r:id="rId12" xr:uid="{BA467D2F-0948-4A82-B49C-B8DCBA7936A0}"/>
-    <hyperlink ref="D27" r:id="rId13" display="Link" xr:uid="{49178A12-AF45-4969-AC8E-49BA3EBADDA9}"/>
-    <hyperlink ref="D17" r:id="rId14" xr:uid="{9689F2B7-24E0-4CC5-A39F-53D7E0370FC8}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{537A3F3C-7C92-42A9-B8B2-F37129F7787F}"/>
-    <hyperlink ref="D18" r:id="rId16" xr:uid="{82909F8B-3A14-4248-8CB2-384756C6E8BE}"/>
-    <hyperlink ref="D28" r:id="rId17" xr:uid="{0D6A5659-9181-49D0-A7D8-101F63076C8A}"/>
-    <hyperlink ref="D11" r:id="rId18" xr:uid="{4AEFCE09-28B7-4C24-82DE-ADAB9CAA43E1}"/>
-    <hyperlink ref="D12" r:id="rId19" xr:uid="{0ED2334F-09CF-437E-82F8-E81D86F288DC}"/>
-    <hyperlink ref="D24" r:id="rId20" xr:uid="{87CB364F-700B-4E81-BC67-3C859C1B7934}"/>
-    <hyperlink ref="D25" r:id="rId21" display="5X High End" xr:uid="{D4CB98E8-7A2B-495D-9E37-8208D21A6270}"/>
-    <hyperlink ref="D26" r:id="rId22" display="6x5x1 Option Shim" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
-    <hyperlink ref="F26" r:id="rId23" display="NB! 200 pcs option is same price" xr:uid="{D98A7A59-4D4C-4589-8C00-1DCF83FFF3E6}"/>
-    <hyperlink ref="F6" r:id="rId24" xr:uid="{5B14FBB6-ADAD-4948-95D7-FBD8C9BC5BB5}"/>
-    <hyperlink ref="D7" r:id="rId25" display="MKS DUET WIFI" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
-    <hyperlink ref="F7" r:id="rId26" display="Mini 12864" xr:uid="{321ACA62-20AB-45F9-A643-EE2EB664C961}"/>
-    <hyperlink ref="D29" r:id="rId27" xr:uid="{53A16D3E-EBE4-45B6-9E87-70111D7D2FFE}"/>
-    <hyperlink ref="F29" r:id="rId28" xr:uid="{2E01C49B-F943-468C-B222-27E06F7C15FC}"/>
-    <hyperlink ref="A31" r:id="rId29" display="Cable Loom - Bowden Path" xr:uid="{73998A44-7105-4A13-A714-12369DB7FB93}"/>
-    <hyperlink ref="D31" r:id="rId30" display="Cable Loom - Bowden Path" xr:uid="{5DD23B84-72DC-46EC-A740-B82AFAD09C94}"/>
-    <hyperlink ref="D30" r:id="rId31" xr:uid="{0C6F2C79-ACBB-4C55-AC21-4895BA685D6B}"/>
+    <hyperlink ref="D25" r:id="rId1" xr:uid="{3773511A-F3AF-4897-B5BB-16FB39A0B508}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{AFC120EB-E75F-4BB8-BC6D-4AA9408DD14D}"/>
+    <hyperlink ref="D23" r:id="rId3" display="Link" xr:uid="{401DDADA-DB79-4416-96CF-3B1D6329769B}"/>
+    <hyperlink ref="D17" r:id="rId4" display="24V Dual Ball" xr:uid="{98BCAD8D-1DD9-49E5-B60D-FB8A39108E71}"/>
+    <hyperlink ref="D16" r:id="rId5" xr:uid="{968A8156-5055-4A5F-97A2-06DF8EA0EB3D}"/>
+    <hyperlink ref="D27" r:id="rId6" display="5 Meter Gates LL" xr:uid="{9F0DE403-B0EC-4933-928F-2806FBCF603A}"/>
+    <hyperlink ref="D22" r:id="rId7" display="Link" xr:uid="{45531F32-6B6C-44D5-9B2A-FB1F259BC9F9}"/>
+    <hyperlink ref="F25" r:id="rId8" display="Keenovo" xr:uid="{C2A02BBB-B317-4856-A562-A30BE2CA0A6C}"/>
+    <hyperlink ref="D19" r:id="rId9" display="8 Bore" xr:uid="{4C50ADBB-FC9C-42E4-8421-5A0C1600DD46}"/>
+    <hyperlink ref="D18" r:id="rId10" display="5 BORE" xr:uid="{43C03DCA-7867-4C9F-B1D0-8588267A1C82}"/>
+    <hyperlink ref="D26" r:id="rId11" xr:uid="{A901DFE1-486C-4AC2-8672-C18618945E04}"/>
+    <hyperlink ref="D24" r:id="rId12" xr:uid="{BA467D2F-0948-4A82-B49C-B8DCBA7936A0}"/>
+    <hyperlink ref="D20" r:id="rId13" display="Link" xr:uid="{49178A12-AF45-4969-AC8E-49BA3EBADDA9}"/>
+    <hyperlink ref="D14" r:id="rId14" xr:uid="{9689F2B7-24E0-4CC5-A39F-53D7E0370FC8}"/>
+    <hyperlink ref="D28" r:id="rId15" xr:uid="{537A3F3C-7C92-42A9-B8B2-F37129F7787F}"/>
+    <hyperlink ref="D8" r:id="rId16" xr:uid="{82909F8B-3A14-4248-8CB2-384756C6E8BE}"/>
+    <hyperlink ref="D29" r:id="rId17" xr:uid="{0D6A5659-9181-49D0-A7D8-101F63076C8A}"/>
+    <hyperlink ref="D21" r:id="rId18" xr:uid="{4AEFCE09-28B7-4C24-82DE-ADAB9CAA43E1}"/>
+    <hyperlink ref="D30" r:id="rId19" xr:uid="{0ED2334F-09CF-437E-82F8-E81D86F288DC}"/>
+    <hyperlink ref="D7" r:id="rId20" xr:uid="{87CB364F-700B-4E81-BC67-3C859C1B7934}"/>
+    <hyperlink ref="D6" r:id="rId21" display="5X High End" xr:uid="{D4CB98E8-7A2B-495D-9E37-8208D21A6270}"/>
+    <hyperlink ref="D5" r:id="rId22" display="6x5x1 Option Shim" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
+    <hyperlink ref="F5" r:id="rId23" display="NB! 200 pcs option is same price" xr:uid="{D98A7A59-4D4C-4589-8C00-1DCF83FFF3E6}"/>
+    <hyperlink ref="F13" r:id="rId24" xr:uid="{5B14FBB6-ADAD-4948-95D7-FBD8C9BC5BB5}"/>
+    <hyperlink ref="D12" r:id="rId25" display="MKS DUET WIFI" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
+    <hyperlink ref="F12" r:id="rId26" display="Mini 12864" xr:uid="{321ACA62-20AB-45F9-A643-EE2EB664C961}"/>
+    <hyperlink ref="D15" r:id="rId27" xr:uid="{53A16D3E-EBE4-45B6-9E87-70111D7D2FFE}"/>
+    <hyperlink ref="F15" r:id="rId28" xr:uid="{2E01C49B-F943-468C-B222-27E06F7C15FC}"/>
+    <hyperlink ref="D10" r:id="rId29" display="Cable Loom - Bowden Path" xr:uid="{5DD23B84-72DC-46EC-A740-B82AFAD09C94}"/>
+    <hyperlink ref="D11" r:id="rId30" xr:uid="{0C6F2C79-ACBB-4C55-AC21-4895BA685D6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId32"/>
-  <drawing r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId31"/>
+  <drawing r:id="rId32"/>
   <tableParts count="1">
-    <tablePart r:id="rId34"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3644,17 +3659,17 @@
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="76" t="s">
         <v>104</v>
       </c>
       <c r="F1" t="s">
@@ -3668,529 +3683,529 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="29">
         <v>2</v>
       </c>
-      <c r="D2" s="95">
+      <c r="D2" s="77">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="29">
         <v>4</v>
       </c>
-      <c r="D3" s="95">
+      <c r="D3" s="77">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="29">
         <v>4</v>
       </c>
-      <c r="D4" s="95">
+      <c r="D4" s="77">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="95">
+      <c r="D5" s="77">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="29">
         <v>2</v>
       </c>
-      <c r="D6" s="95">
+      <c r="D6" s="77">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="29">
         <v>11</v>
       </c>
-      <c r="D7" s="95">
+      <c r="D7" s="77">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="29">
         <v>15</v>
       </c>
-      <c r="D8" s="95">
+      <c r="D8" s="77">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="95">
+      <c r="D9" s="77">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="29">
         <v>9</v>
       </c>
-      <c r="D10" s="95">
+      <c r="D10" s="77">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="29">
         <v>5</v>
       </c>
-      <c r="D11" s="95">
+      <c r="D11" s="77">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="29">
         <v>8</v>
       </c>
-      <c r="D12" s="95">
+      <c r="D12" s="77">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" s="32">
+      <c r="C13" s="29">
         <v>2</v>
       </c>
-      <c r="D13" s="95">
+      <c r="D13" s="77">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="29">
         <v>5</v>
       </c>
-      <c r="D14" s="95">
+      <c r="D14" s="77">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="29">
         <v>5</v>
       </c>
-      <c r="D15" s="95">
+      <c r="D15" s="77">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="95">
+      <c r="D16" s="77">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="29">
         <v>6</v>
       </c>
-      <c r="D17" s="95">
+      <c r="D17" s="77">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="29">
         <v>2</v>
       </c>
-      <c r="D18" s="95">
+      <c r="D18" s="77">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="29">
         <v>1</v>
       </c>
-      <c r="D19" s="95">
+      <c r="D19" s="77">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" s="32">
+      <c r="B20" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="29">
         <v>3</v>
       </c>
-      <c r="D20" s="95">
+      <c r="D20" s="77">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C21" s="32">
+      <c r="B21" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="29">
         <v>1</v>
       </c>
-      <c r="D21" s="95">
+      <c r="D21" s="77">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="29">
         <v>1</v>
       </c>
-      <c r="D22" s="95">
+      <c r="D22" s="77">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="29">
         <v>28</v>
       </c>
-      <c r="D23" s="95">
+      <c r="D23" s="77">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="29">
         <v>6</v>
       </c>
-      <c r="D24" s="95">
+      <c r="D24" s="77">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="29">
         <v>50</v>
       </c>
-      <c r="D25" s="95">
+      <c r="D25" s="77">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C26" s="32">
+      <c r="B26" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" s="29">
         <v>63</v>
       </c>
-      <c r="D26" s="95">
+      <c r="D26" s="77">
         <v>70</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>197</v>
+      <c r="E26" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="29">
         <v>143</v>
       </c>
-      <c r="D27" s="95">
+      <c r="D27" s="77">
         <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="29">
         <v>200</v>
       </c>
-      <c r="D28" s="95">
+      <c r="D28" s="77">
         <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="29">
         <v>142</v>
       </c>
-      <c r="D29" s="95">
+      <c r="D29" s="77">
         <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="29">
         <v>8</v>
       </c>
-      <c r="D30" s="95">
+      <c r="D30" s="77">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="29">
         <v>1</v>
       </c>
-      <c r="D31" s="95">
+      <c r="D31" s="77">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="29">
         <v>2</v>
       </c>
-      <c r="D32" s="95">
+      <c r="D32" s="77">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="29">
         <v>2</v>
       </c>
-      <c r="D33" s="95">
+      <c r="D33" s="77">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="29">
         <v>18</v>
       </c>
-      <c r="D34" s="95">
+      <c r="D34" s="77">
         <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="29">
         <v>8</v>
       </c>
-      <c r="D35" s="95">
+      <c r="D35" s="77">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C36" s="32">
+      <c r="B36" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="29">
         <v>4</v>
       </c>
-      <c r="D36" s="95">
+      <c r="D36" s="77">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="69" t="s">
+      <c r="A37" s="63" t="s">
         <v>146</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="97">
+      <c r="B37" s="64"/>
+      <c r="C37" s="79">
         <f>SUM(C2:C36)</f>
         <v>782</v>
       </c>
-      <c r="D37" s="98">
+      <c r="D37" s="80">
         <f>SUM(D2:D36)</f>
         <v>806</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="99">
+      <c r="B38" s="6"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="81">
         <v>0.1</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="28">
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="25">
         <f>D37*D38</f>
         <v>80.600000000000009</v>
       </c>

</xml_diff>

<commit_message>
panel cut pattern 250
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-Baby BOM.xlsx
+++ b/Document Library/Bill Of Materials/V-Baby BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-Baby CoreXY/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2087" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DE62A0DF-03CB-4643-A9C9-49C7A4EC3BBB}"/>
+  <xr:revisionPtr revIDLastSave="2089" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EAC3A91D-58C3-4C27-9FED-5B6BD30E5502}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpenBuild Part List" sheetId="1" r:id="rId1"/>
@@ -1403,12 +1403,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1419,6 +1413,12 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
@@ -2339,19 +2339,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2379,13 +2379,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="20"/>
-      <c r="F2" s="133" t="s">
+      <c r="F2" s="143" t="s">
         <v>144</v>
       </c>
       <c r="G2" s="41"/>
@@ -2393,7 +2393,7 @@
       <c r="I2" s="43"/>
       <c r="J2" s="59"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>7</v>
       </c>
@@ -2410,13 +2410,13 @@
         <f>D3*310</f>
         <v>1240</v>
       </c>
-      <c r="F3" s="134"/>
+      <c r="F3" s="144"/>
       <c r="G3" s="41"/>
       <c r="H3" s="50"/>
       <c r="I3" s="15"/>
       <c r="J3" s="60"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>10</v>
       </c>
@@ -2433,13 +2433,13 @@
         <f>D4*350</f>
         <v>1400</v>
       </c>
-      <c r="F4" s="134"/>
+      <c r="F4" s="144"/>
       <c r="G4" s="41"/>
       <c r="H4" s="51"/>
       <c r="I4" s="43"/>
       <c r="J4" s="59"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>13</v>
       </c>
@@ -2456,13 +2456,13 @@
         <f>D5*340</f>
         <v>1700</v>
       </c>
-      <c r="F5" s="134"/>
+      <c r="F5" s="144"/>
       <c r="G5" s="41"/>
       <c r="H5" s="50"/>
       <c r="I5" s="15"/>
       <c r="J5" s="60"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>16</v>
       </c>
@@ -2479,25 +2479,25 @@
         <f>D6*295</f>
         <v>295</v>
       </c>
-      <c r="F6" s="134"/>
+      <c r="F6" s="144"/>
       <c r="G6" s="41"/>
       <c r="H6" s="51"/>
       <c r="I6" s="43"/>
       <c r="J6" s="59"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="48"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="134"/>
+      <c r="F7" s="144"/>
       <c r="G7" s="41"/>
       <c r="H7" s="26"/>
       <c r="I7" s="6"/>
       <c r="J7" s="60"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
         <v>18</v>
       </c>
@@ -2514,13 +2514,13 @@
         <f>D8*290</f>
         <v>290</v>
       </c>
-      <c r="F8" s="134"/>
+      <c r="F8" s="144"/>
       <c r="G8" s="41"/>
       <c r="H8" s="51"/>
       <c r="I8" s="43"/>
       <c r="J8" s="59"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>21</v>
       </c>
@@ -2537,13 +2537,13 @@
         <f>D9*350</f>
         <v>700</v>
       </c>
-      <c r="F9" s="134"/>
+      <c r="F9" s="144"/>
       <c r="G9" s="41"/>
       <c r="H9" s="50"/>
       <c r="I9" s="15"/>
       <c r="J9" s="60"/>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
         <v>24</v>
       </c>
@@ -2558,7 +2558,7 @@
         <f>SUM(E3:E9)</f>
         <v>5625</v>
       </c>
-      <c r="F10" s="134"/>
+      <c r="F10" s="144"/>
       <c r="G10" s="41"/>
       <c r="H10" s="52" t="s">
         <v>27</v>
@@ -2570,13 +2570,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="134"/>
+      <c r="F11" s="144"/>
       <c r="G11" s="41"/>
       <c r="H11" s="26" t="s">
         <v>28</v>
@@ -2586,7 +2586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>29</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="21"/>
-      <c r="F12" s="134"/>
+      <c r="F12" s="144"/>
       <c r="G12" s="41"/>
       <c r="H12" s="52" t="s">
         <v>31</v>
@@ -2612,19 +2612,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="48"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="134"/>
+      <c r="F13" s="144"/>
       <c r="G13" s="41"/>
       <c r="H13" s="26"/>
       <c r="I13" s="62"/>
       <c r="J13" s="60"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49" t="s">
         <v>32</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="F14" s="134"/>
+      <c r="F14" s="144"/>
       <c r="G14" s="41"/>
       <c r="H14" s="52" t="s">
         <v>35</v>
@@ -2650,7 +2650,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>36</v>
       </c>
@@ -2669,11 +2669,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>37</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>38</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>39</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>41</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>80.600000000000009</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="38" t="s">
         <v>147</v>
       </c>
@@ -2803,14 +2803,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" style="73" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="73" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="75" t="s">
         <v>153</v>
       </c>
@@ -2821,7 +2821,7 @@
       <c r="F1" s="76"/>
       <c r="G1" s="78"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="79"/>
       <c r="B2" s="6"/>
       <c r="C2" s="80"/>
@@ -2830,7 +2830,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" s="74" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="74" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="81" t="s">
         <v>154</v>
       </c>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="G3" s="85"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
         <v>168</v>
       </c>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
         <v>169</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>170</v>
       </c>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
         <v>18</v>
       </c>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>21</v>
       </c>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
         <v>16</v>
       </c>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="79"/>
       <c r="B10" s="6"/>
       <c r="C10" s="80"/>
@@ -2986,7 +2986,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" s="74" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" s="74" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="81" t="s">
         <v>161</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="F11" s="82"/>
       <c r="G11" s="85"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
         <v>160</v>
       </c>
@@ -3008,7 +3008,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="86" t="s">
         <v>162</v>
       </c>
@@ -3023,7 +3023,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
         <v>168</v>
       </c>
@@ -3043,7 +3043,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
         <v>169</v>
       </c>
@@ -3065,7 +3065,7 @@
       </c>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="79" t="s">
         <v>170</v>
       </c>
@@ -3085,7 +3085,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
         <v>18</v>
       </c>
@@ -3101,7 +3101,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="79" t="s">
         <v>21</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="90" t="s">
         <v>16</v>
       </c>
@@ -3133,7 +3133,7 @@
       <c r="F19" s="94"/>
       <c r="G19" s="95"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="80"/>
@@ -3142,17 +3142,17 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>167</v>
       </c>
@@ -3175,23 +3175,21 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.26953125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="126"/>
       <c r="B1" s="76"/>
       <c r="C1" s="76"/>
@@ -3200,7 +3198,7 @@
       <c r="F1" s="128"/>
       <c r="G1" s="129"/>
     </row>
-    <row r="2" spans="1:8" ht="27" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:8" ht="27.75" x14ac:dyDescent="0.5">
       <c r="A2" s="130"/>
       <c r="B2" s="103"/>
       <c r="C2" s="112"/>
@@ -3211,7 +3209,7 @@
       <c r="F2" s="101"/>
       <c r="G2" s="131"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3220,34 +3218,34 @@
       <c r="F3" s="98"/>
       <c r="G3" s="132"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="138" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="136" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="139"/>
-      <c r="C4" s="139" t="s">
+      <c r="B4" s="137"/>
+      <c r="C4" s="137" t="s">
         <v>208</v>
       </c>
-      <c r="D4" s="140"/>
-      <c r="E4" s="141">
+      <c r="D4" s="138"/>
+      <c r="E4" s="139">
         <v>334</v>
       </c>
-      <c r="G4" s="135"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="136" t="s">
+      <c r="G4" s="133"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="137" t="s">
+      <c r="B5" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="137" t="s">
+      <c r="C5" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="137" t="s">
+      <c r="D5" s="135" t="s">
         <v>189</v>
       </c>
-      <c r="E5" s="137" t="s">
+      <c r="E5" s="135" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="113" t="s">
@@ -3257,7 +3255,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>179</v>
       </c>
@@ -3278,7 +3276,7 @@
       </c>
       <c r="G6" s="104"/>
     </row>
-    <row r="7" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>89</v>
       </c>
@@ -3297,7 +3295,7 @@
       <c r="F7" s="107"/>
       <c r="G7" s="106"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>87</v>
       </c>
@@ -3316,7 +3314,7 @@
       <c r="F8" s="111"/>
       <c r="G8" s="104"/>
     </row>
-    <row r="9" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>68</v>
       </c>
@@ -3336,7 +3334,7 @@
       <c r="G9" s="104"/>
       <c r="H9" s="102"/>
     </row>
-    <row r="10" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>50</v>
       </c>
@@ -3356,7 +3354,7 @@
       <c r="G10" s="104"/>
       <c r="H10" s="102"/>
     </row>
-    <row r="11" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>192</v>
       </c>
@@ -3376,7 +3374,7 @@
       <c r="G11" s="104"/>
       <c r="H11" s="102"/>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>196</v>
       </c>
@@ -3395,7 +3393,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="104"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
@@ -3414,7 +3412,7 @@
       <c r="F13" s="111"/>
       <c r="G13" s="104"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>67</v>
       </c>
@@ -3433,7 +3431,7 @@
       <c r="F14" s="15"/>
       <c r="G14" s="104"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>182</v>
       </c>
@@ -3456,7 +3454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>200</v>
       </c>
@@ -3475,7 +3473,7 @@
       <c r="F16" s="15"/>
       <c r="G16" s="104"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -3494,7 +3492,7 @@
       <c r="F17" s="15"/>
       <c r="G17" s="104"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>44</v>
       </c>
@@ -3513,7 +3511,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="104"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>81</v>
       </c>
@@ -3532,7 +3530,7 @@
       <c r="F19" s="15"/>
       <c r="G19" s="104"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>84</v>
       </c>
@@ -3551,7 +3549,7 @@
       <c r="F20" s="15"/>
       <c r="G20" s="104"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>92</v>
       </c>
@@ -3570,7 +3568,7 @@
       <c r="F21" s="15"/>
       <c r="G21" s="104"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>53</v>
       </c>
@@ -3589,7 +3587,7 @@
       <c r="F22" s="111"/>
       <c r="G22" s="104"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>74</v>
       </c>
@@ -3608,7 +3606,7 @@
       <c r="F23" s="15"/>
       <c r="G23" s="104"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>71</v>
       </c>
@@ -3627,7 +3625,7 @@
       <c r="F24" s="15"/>
       <c r="G24" s="104"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>64</v>
       </c>
@@ -3646,7 +3644,7 @@
       <c r="F25" s="115"/>
       <c r="G25" s="104"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>58</v>
       </c>
@@ -3669,7 +3667,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>61</v>
       </c>
@@ -3688,7 +3686,7 @@
       <c r="F27" s="115"/>
       <c r="G27" s="104"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>77</v>
       </c>
@@ -3707,7 +3705,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="104"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>95</v>
       </c>
@@ -3726,7 +3724,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="104"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>55</v>
       </c>
@@ -3745,7 +3743,7 @@
       <c r="F30" s="116"/>
       <c r="G30" s="104"/>
     </row>
-    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="108" t="s">
         <v>97</v>
       </c>
@@ -3759,14 +3757,14 @@
       <c r="F31" s="65"/>
       <c r="G31" s="65"/>
     </row>
-    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="142" t="s">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="140" t="s">
         <v>209</v>
       </c>
-      <c r="B32" s="143"/>
-      <c r="C32" s="143"/>
-      <c r="D32" s="143"/>
-      <c r="E32" s="144">
+      <c r="B32" s="141"/>
+      <c r="C32" s="141"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="142">
         <f>E4+E31</f>
         <v>795</v>
       </c>
@@ -3819,20 +3817,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -3855,7 +3853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>99</v>
       </c>
@@ -3869,7 +3867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>101</v>
       </c>
@@ -3883,7 +3881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>102</v>
       </c>
@@ -3897,7 +3895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>104</v>
       </c>
@@ -3911,7 +3909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>105</v>
       </c>
@@ -3925,7 +3923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>107</v>
       </c>
@@ -3939,7 +3937,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>108</v>
       </c>
@@ -3953,7 +3951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>110</v>
       </c>
@@ -3967,7 +3965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>111</v>
       </c>
@@ -3981,7 +3979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>112</v>
       </c>
@@ -3995,7 +3993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>113</v>
       </c>
@@ -4009,7 +4007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>151</v>
       </c>
@@ -4023,7 +4021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>114</v>
       </c>
@@ -4037,7 +4035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>116</v>
       </c>
@@ -4051,7 +4049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>117</v>
       </c>
@@ -4065,7 +4063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>118</v>
       </c>
@@ -4079,7 +4077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>119</v>
       </c>
@@ -4093,7 +4091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>120</v>
       </c>
@@ -4107,7 +4105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>121</v>
       </c>
@@ -4121,7 +4119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>122</v>
       </c>
@@ -4135,7 +4133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>123</v>
       </c>
@@ -4149,7 +4147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>124</v>
       </c>
@@ -4163,7 +4161,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>125</v>
       </c>
@@ -4177,7 +4175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>126</v>
       </c>
@@ -4191,7 +4189,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>128</v>
       </c>
@@ -4208,7 +4206,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>129</v>
       </c>
@@ -4222,7 +4220,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>131</v>
       </c>
@@ -4236,7 +4234,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>132</v>
       </c>
@@ -4250,7 +4248,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>133</v>
       </c>
@@ -4264,7 +4262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>134</v>
       </c>
@@ -4278,7 +4276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
         <v>135</v>
       </c>
@@ -4292,7 +4290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>136</v>
       </c>
@@ -4306,7 +4304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>137</v>
       </c>
@@ -4320,7 +4318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>138</v>
       </c>
@@ -4334,7 +4332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>139</v>
       </c>
@@ -4348,7 +4346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="63" t="s">
         <v>140</v>
       </c>
@@ -4362,7 +4360,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="26" t="s">
         <v>141</v>
       </c>
@@ -4372,7 +4370,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>142</v>
       </c>
@@ -4398,14 +4396,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
changed from mks board to btt is better
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-Baby BOM.xlsx
+++ b/Document Library/Bill Of Materials/V-Baby BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-Baby CoreXY/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2227" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E4DE46BE-AE9F-44A5-A7BB-848511CF3C21}"/>
+  <xr:revisionPtr revIDLastSave="2228" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{07B600EE-DBB2-4D61-A886-1D1A4F73372A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpenBuild Part List" sheetId="1" r:id="rId1"/>
@@ -2409,7 +2409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -3245,8 +3245,8 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3924,7 +3924,7 @@
     <hyperlink ref="D8" r:id="rId20" xr:uid="{D4CB98E8-7A2B-495D-9E37-8208D21A6270}"/>
     <hyperlink ref="D6" r:id="rId21" display="6x5x1 Option Shim" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
     <hyperlink ref="F6" r:id="rId22" display="NB! 200 pcs option is same price" xr:uid="{D98A7A59-4D4C-4589-8C00-1DCF83FFF3E6}"/>
-    <hyperlink ref="D17" r:id="rId23" display="BTT DUET WIFI Clone" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
+    <hyperlink ref="D17" r:id="rId23" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
     <hyperlink ref="D19" r:id="rId24" xr:uid="{53A16D3E-EBE4-45B6-9E87-70111D7D2FFE}"/>
     <hyperlink ref="F19" r:id="rId25" xr:uid="{2E01C49B-F943-468C-B222-27E06F7C15FC}"/>
     <hyperlink ref="D15" r:id="rId26" display="Cable Loom - Bowden Path" xr:uid="{5DD23B84-72DC-46EC-A740-B82AFAD09C94}"/>

</xml_diff>

<commit_message>
Added bolt for Z drive gear
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-Baby BOM.xlsx
+++ b/Document Library/Bill Of Materials/V-Baby BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-Baby CoreXY/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2452" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A13F721A-D915-4FEE-BFE8-563DFE4A02F4}"/>
+  <xr:revisionPtr revIDLastSave="2465" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{114B7AA6-BC44-4140-96A5-E6F293C7B3B4}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="243">
   <si>
     <t>Exstrusions</t>
   </si>
@@ -709,9 +709,6 @@
     <t>Fan Part Cooling</t>
   </si>
   <si>
-    <t>GT2 Motor Pulley 5Bore</t>
-  </si>
-  <si>
     <t>Stepper motor 1.8 Amp</t>
   </si>
   <si>
@@ -736,9 +733,6 @@
     <t>1x10</t>
   </si>
   <si>
-    <t>Z Drive Bearings</t>
-  </si>
-  <si>
     <t>625RS Bearings</t>
   </si>
   <si>
@@ -748,13 +742,28 @@
     <t>Dragonfly Phateus Color: BMO</t>
   </si>
   <si>
-    <t>XY Idler Bearing shafts</t>
-  </si>
-  <si>
     <t>Bearing shafts 5mm</t>
   </si>
   <si>
     <t>5mm Length: 35mm 6PC</t>
+  </si>
+  <si>
+    <t>Belt Motor Pulley GT2</t>
+  </si>
+  <si>
+    <t>Belt Idler Bearing shafts</t>
+  </si>
+  <si>
+    <t>Z Drive Gear Bearings</t>
+  </si>
+  <si>
+    <t>Z Drive Gear Pulley Bolt</t>
+  </si>
+  <si>
+    <t>Bolt for the Gear Pulleys</t>
+  </si>
+  <si>
+    <t>M5 Length: 55mm</t>
   </si>
 </sst>
 </file>
@@ -1547,22 +1556,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
@@ -2153,9 +2162,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1070DF90-74AC-4245-AA46-2FAD63F74767}" name="Table1" displayName="Table1" ref="A6:G34" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" headerRowCellStyle="Accent1">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:G34">
-    <sortCondition ref="A6:A34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1070DF90-74AC-4245-AA46-2FAD63F74767}" name="Table1" displayName="Table1" ref="A6:G35" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" headerRowCellStyle="Accent1">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:G35">
+    <sortCondition ref="A6:A35"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AB8C8187-911D-4248-8608-1F70796FF7C8}" name="Column1" headerRowDxfId="11"/>
@@ -2544,7 +2553,7 @@
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="154" t="s">
+      <c r="F8" s="155" t="s">
         <v>116</v>
       </c>
       <c r="G8" s="40"/>
@@ -2569,7 +2578,7 @@
         <f>D9*310</f>
         <v>1240</v>
       </c>
-      <c r="F9" s="155"/>
+      <c r="F9" s="156"/>
       <c r="G9" s="40"/>
       <c r="H9" s="49"/>
       <c r="I9" s="15"/>
@@ -2592,7 +2601,7 @@
         <f>D10*350</f>
         <v>1400</v>
       </c>
-      <c r="F10" s="155"/>
+      <c r="F10" s="156"/>
       <c r="G10" s="40"/>
       <c r="H10" s="50"/>
       <c r="I10" s="42"/>
@@ -2615,7 +2624,7 @@
         <f>D11*340</f>
         <v>1700</v>
       </c>
-      <c r="F11" s="155"/>
+      <c r="F11" s="156"/>
       <c r="G11" s="40"/>
       <c r="H11" s="49"/>
       <c r="I11" s="15"/>
@@ -2638,7 +2647,7 @@
         <f>D12*295</f>
         <v>295</v>
       </c>
-      <c r="F12" s="155"/>
+      <c r="F12" s="156"/>
       <c r="G12" s="40"/>
       <c r="H12" s="50"/>
       <c r="I12" s="42"/>
@@ -2650,7 +2659,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="155"/>
+      <c r="F13" s="156"/>
       <c r="G13" s="40"/>
       <c r="H13" s="26"/>
       <c r="I13" s="6"/>
@@ -2673,7 +2682,7 @@
         <f>D14*290</f>
         <v>290</v>
       </c>
-      <c r="F14" s="155"/>
+      <c r="F14" s="156"/>
       <c r="G14" s="40"/>
       <c r="H14" s="50"/>
       <c r="I14" s="42"/>
@@ -2696,7 +2705,7 @@
         <f>D15*350</f>
         <v>700</v>
       </c>
-      <c r="F15" s="155"/>
+      <c r="F15" s="156"/>
       <c r="G15" s="40"/>
       <c r="H15" s="49" t="s">
         <v>186</v>
@@ -2719,7 +2728,7 @@
         <f>SUM(E9:E15)</f>
         <v>5625</v>
       </c>
-      <c r="F16" s="155"/>
+      <c r="F16" s="156"/>
       <c r="G16" s="40"/>
       <c r="H16" s="51" t="s">
         <v>185</v>
@@ -2737,7 +2746,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="155"/>
+      <c r="F17" s="156"/>
       <c r="G17" s="40"/>
       <c r="H17" s="26" t="s">
         <v>27</v>
@@ -2761,7 +2770,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="21"/>
-      <c r="F18" s="155"/>
+      <c r="F18" s="156"/>
       <c r="G18" s="40"/>
       <c r="H18" s="51" t="s">
         <v>30</v>
@@ -2779,7 +2788,7 @@
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="155"/>
+      <c r="F19" s="156"/>
       <c r="G19" s="40"/>
       <c r="H19" s="26"/>
       <c r="I19" s="61"/>
@@ -2799,7 +2808,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="21"/>
-      <c r="F20" s="155"/>
+      <c r="F20" s="156"/>
       <c r="G20" s="40"/>
       <c r="H20" s="51" t="s">
         <v>34</v>
@@ -2865,8 +2874,8 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="146">
-        <f>'Component Part List'!$E$35</f>
-        <v>503.5</v>
+        <f>'Component Part List'!$E$36</f>
+        <v>509.5</v>
       </c>
       <c r="G25" s="41"/>
       <c r="H25" s="26" t="s">
@@ -2874,8 +2883,8 @@
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="146">
-        <f>'Component Part List'!$E$35</f>
-        <v>503.5</v>
+        <f>'Component Part List'!$E$36</f>
+        <v>509.5</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2929,7 +2938,7 @@
       <c r="E28" s="38"/>
       <c r="F28" s="34">
         <f>SUM(F24:F27)</f>
-        <v>863.5</v>
+        <v>869.5</v>
       </c>
       <c r="G28" s="41"/>
       <c r="H28" s="52" t="s">
@@ -2938,7 +2947,7 @@
       <c r="I28" s="53"/>
       <c r="J28" s="54">
         <f>SUM(J24:J27)</f>
-        <v>742.1</v>
+        <v>748.1</v>
       </c>
     </row>
   </sheetData>
@@ -3327,7 +3336,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3425,7 +3434,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="92"/>
-      <c r="G6" s="156"/>
+      <c r="G6" s="153"/>
     </row>
     <row r="7" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -3486,424 +3495,424 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>150</v>
+        <v>238</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="C10" s="91">
-        <v>80</v>
-      </c>
-      <c r="D10" s="105" t="s">
-        <v>204</v>
-      </c>
-      <c r="E10" s="102">
-        <v>15</v>
-      </c>
-      <c r="F10" s="96"/>
+        <v>235</v>
+      </c>
+      <c r="C10" s="91" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="154" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" s="103">
+        <v>3</v>
+      </c>
+      <c r="F10" s="15"/>
       <c r="G10" s="103"/>
     </row>
     <row r="11" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" s="91" t="s">
-        <v>182</v>
+        <v>166</v>
+      </c>
+      <c r="C11" s="91">
+        <v>80</v>
       </c>
       <c r="D11" s="105" t="s">
-        <v>218</v>
-      </c>
-      <c r="E11" s="103">
-        <v>13</v>
-      </c>
-      <c r="F11" s="15"/>
+        <v>204</v>
+      </c>
+      <c r="E11" s="102">
+        <v>15</v>
+      </c>
+      <c r="F11" s="96"/>
       <c r="G11" s="103"/>
     </row>
     <row r="12" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="C12" s="91" t="s">
-        <v>181</v>
+        <v>68</v>
+      </c>
+      <c r="C12" s="91">
+        <v>2</v>
       </c>
       <c r="D12" s="105" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E12" s="103">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="103"/>
     </row>
     <row r="13" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="91">
-        <v>1</v>
+        <v>183</v>
+      </c>
+      <c r="C13" s="91" t="s">
+        <v>182</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E13" s="103">
-        <v>2.5</v>
+        <v>13</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="103"/>
     </row>
     <row r="14" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>161</v>
+      <c r="A14" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" s="91">
-        <v>1</v>
+        <v>184</v>
+      </c>
+      <c r="C14" s="91" t="s">
+        <v>181</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>160</v>
+        <v>217</v>
       </c>
       <c r="E14" s="103">
-        <v>2.5</v>
+        <v>19</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="103"/>
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="C15" s="91">
         <v>1</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="E15" s="103">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="103"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>42</v>
+      <c r="A16" s="14" t="s">
+        <v>161</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="C16" s="91">
         <v>1</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="E16" s="103">
-        <v>60</v>
-      </c>
-      <c r="F16" s="96"/>
+        <v>2.5</v>
+      </c>
+      <c r="F16" s="15"/>
       <c r="G16" s="103"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>59</v>
+        <v>165</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C17" s="91">
         <v>1</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E17" s="103">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="103"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>222</v>
+        <v>42</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="C18" s="91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="E18" s="103">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F18" s="96"/>
       <c r="G18" s="103"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>221</v>
+        <v>59</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="C19" s="91">
         <v>1</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="E19" s="103">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="103"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20" s="91">
         <v>2</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="E20" s="103">
         <v>10</v>
       </c>
-      <c r="F20" s="15"/>
+      <c r="F20" s="96"/>
       <c r="G20" s="103"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C21" s="91">
+        <v>1</v>
+      </c>
+      <c r="D21" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="E21" s="103">
         <v>2</v>
-      </c>
-      <c r="D21" s="105" t="s">
-        <v>208</v>
-      </c>
-      <c r="E21" s="103">
-        <v>11</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="103"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>155</v>
+        <v>43</v>
       </c>
       <c r="C22" s="91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="105" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="E22" s="103">
-        <v>30</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="G22" s="103">
-        <v>16</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="103"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C23" s="91">
         <v>1</v>
       </c>
       <c r="D23" s="105" t="s">
-        <v>236</v>
+        <v>156</v>
       </c>
       <c r="E23" s="103">
-        <v>73</v>
-      </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="103"/>
+        <v>30</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" s="103">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>226</v>
+        <v>167</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="C24" s="91" t="s">
-        <v>228</v>
+        <v>168</v>
+      </c>
+      <c r="C24" s="91">
+        <v>1</v>
       </c>
       <c r="D24" s="105" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E24" s="103">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="103"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="108" t="s">
-        <v>47</v>
+        <v>225</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>224</v>
       </c>
       <c r="C25" s="91" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D25" s="105" t="s">
-        <v>169</v>
+        <v>226</v>
       </c>
       <c r="E25" s="103">
-        <v>4</v>
-      </c>
-      <c r="F25" s="96"/>
+        <v>30</v>
+      </c>
+      <c r="F25" s="15"/>
       <c r="G25" s="103"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="91">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="B26" s="108" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="91" t="s">
+        <v>228</v>
       </c>
       <c r="D26" s="105" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="E26" s="103">
-        <v>8.5</v>
-      </c>
-      <c r="F26" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="F26" s="96"/>
       <c r="G26" s="103"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C27" s="91">
         <v>1</v>
       </c>
       <c r="D27" s="105" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E27" s="103">
-        <v>20</v>
+        <v>8.5</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="103"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C28" s="91">
         <v>1</v>
       </c>
       <c r="D28" s="105" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E28" s="103">
-        <v>2</v>
-      </c>
-      <c r="F28" s="100"/>
+        <v>20</v>
+      </c>
+      <c r="F28" s="15"/>
       <c r="G28" s="103"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C29" s="91">
         <v>1</v>
       </c>
       <c r="D29" s="105" t="s">
-        <v>230</v>
+        <v>58</v>
       </c>
       <c r="E29" s="103">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="F29" s="100"/>
       <c r="G29" s="103"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" s="91">
         <v>1</v>
       </c>
       <c r="D30" s="105" t="s">
-        <v>55</v>
+        <v>229</v>
       </c>
       <c r="E30" s="103">
-        <v>3.5</v>
+        <v>40</v>
       </c>
       <c r="F30" s="100"/>
       <c r="G30" s="103"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>237</v>
+        <v>53</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="C31" s="91" t="s">
-        <v>229</v>
-      </c>
-      <c r="D31" s="157" t="s">
-        <v>239</v>
+        <v>54</v>
+      </c>
+      <c r="C31" s="91">
+        <v>1</v>
+      </c>
+      <c r="D31" s="105" t="s">
+        <v>55</v>
       </c>
       <c r="E31" s="103">
-        <v>3</v>
-      </c>
-      <c r="F31" s="148"/>
+        <v>3.5</v>
+      </c>
+      <c r="F31" s="157"/>
       <c r="G31" s="103"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3917,7 +3926,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E32" s="103">
         <v>8.5</v>
@@ -3927,16 +3936,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="C33" s="91" t="s">
+        <v>231</v>
+      </c>
+      <c r="D33" s="147" t="s">
         <v>233</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="C33" s="91" t="s">
-        <v>232</v>
-      </c>
-      <c r="D33" s="147" t="s">
-        <v>235</v>
       </c>
       <c r="E33" s="103">
         <v>19</v>
@@ -3946,89 +3955,109 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="C34" s="91">
+        <v>1</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="E34" s="103">
+        <v>6</v>
+      </c>
+      <c r="F34" s="15"/>
+      <c r="G34" s="103"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="109" t="s">
+      <c r="B35" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="107">
+      <c r="C35" s="107">
         <v>1</v>
       </c>
-      <c r="D34" s="106" t="s">
+      <c r="D35" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="104">
+      <c r="E35" s="104">
         <v>14</v>
       </c>
-      <c r="F34" s="101"/>
-      <c r="G34" s="104"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="93" t="s">
+      <c r="F35" s="101"/>
+      <c r="G35" s="104"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="94"/>
-      <c r="C35" s="94"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="95">
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="95">
         <f>SUBTOTAL(109,Table1[[#All],[Column5]])</f>
-        <v>503.5</v>
-      </c>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="124" t="s">
+        <v>509.5</v>
+      </c>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="124" t="s">
         <v>174</v>
       </c>
-      <c r="B36" s="125"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="126">
-        <f>E4+E35</f>
-        <v>837.5</v>
+      <c r="B37" s="125"/>
+      <c r="C37" s="125"/>
+      <c r="D37" s="125"/>
+      <c r="E37" s="126">
+        <f>E4+E36</f>
+        <v>843.5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D29" r:id="rId1" display="220V/110V" xr:uid="{3773511A-F3AF-4897-B5BB-16FB39A0B508}"/>
-    <hyperlink ref="D18" r:id="rId2" xr:uid="{AFC120EB-E75F-4BB8-BC6D-4AA9408DD14D}"/>
-    <hyperlink ref="D27" r:id="rId3" display="Link" xr:uid="{401DDADA-DB79-4416-96CF-3B1D6329769B}"/>
-    <hyperlink ref="D20" r:id="rId4" display="24V Dual Ball" xr:uid="{98BCAD8D-1DD9-49E5-B60D-FB8A39108E71}"/>
-    <hyperlink ref="D12" r:id="rId5" xr:uid="{9F0DE403-B0EC-4933-928F-2806FBCF603A}"/>
-    <hyperlink ref="D26" r:id="rId6" display="Link" xr:uid="{45531F32-6B6C-44D5-9B2A-FB1F259BC9F9}"/>
-    <hyperlink ref="D21" r:id="rId7" xr:uid="{43C03DCA-7867-4C9F-B1D0-8588267A1C82}"/>
-    <hyperlink ref="D30" r:id="rId8" xr:uid="{A901DFE1-486C-4AC2-8672-C18618945E04}"/>
-    <hyperlink ref="D28" r:id="rId9" xr:uid="{BA467D2F-0948-4A82-B49C-B8DCBA7936A0}"/>
-    <hyperlink ref="D24" r:id="rId10" xr:uid="{49178A12-AF45-4969-AC8E-49BA3EBADDA9}"/>
-    <hyperlink ref="D23" r:id="rId11" xr:uid="{537A3F3C-7C92-42A9-B8B2-F37129F7787F}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{82909F8B-3A14-4248-8CB2-384756C6E8BE}"/>
-    <hyperlink ref="D25" r:id="rId13" display="6Pcs Endstops" xr:uid="{4AEFCE09-28B7-4C24-82DE-ADAB9CAA43E1}"/>
-    <hyperlink ref="D34" r:id="rId14" xr:uid="{0ED2334F-09CF-437E-82F8-E81D86F288DC}"/>
-    <hyperlink ref="D10" r:id="rId15" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
-    <hyperlink ref="D16" r:id="rId16" display="MKS DUET WIFI Clone" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
-    <hyperlink ref="D22" r:id="rId17" xr:uid="{53A16D3E-EBE4-45B6-9E87-70111D7D2FFE}"/>
-    <hyperlink ref="F22" r:id="rId18" xr:uid="{2E01C49B-F943-468C-B222-27E06F7C15FC}"/>
-    <hyperlink ref="D14" r:id="rId19" display="Cable Loom - Bowden Path" xr:uid="{5DD23B84-72DC-46EC-A740-B82AFAD09C94}"/>
-    <hyperlink ref="D15" r:id="rId20" xr:uid="{0C6F2C79-ACBB-4C55-AC21-4895BA685D6B}"/>
-    <hyperlink ref="D17" r:id="rId21" xr:uid="{9689F2B7-24E0-4CC5-A39F-53D7E0370FC8}"/>
+    <hyperlink ref="D30" r:id="rId1" display="220V/110V" xr:uid="{3773511A-F3AF-4897-B5BB-16FB39A0B508}"/>
+    <hyperlink ref="D20" r:id="rId2" xr:uid="{AFC120EB-E75F-4BB8-BC6D-4AA9408DD14D}"/>
+    <hyperlink ref="D28" r:id="rId3" display="Link" xr:uid="{401DDADA-DB79-4416-96CF-3B1D6329769B}"/>
+    <hyperlink ref="D22" r:id="rId4" display="24V Dual Ball" xr:uid="{98BCAD8D-1DD9-49E5-B60D-FB8A39108E71}"/>
+    <hyperlink ref="D14" r:id="rId5" xr:uid="{9F0DE403-B0EC-4933-928F-2806FBCF603A}"/>
+    <hyperlink ref="D27" r:id="rId6" display="Link" xr:uid="{45531F32-6B6C-44D5-9B2A-FB1F259BC9F9}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{43C03DCA-7867-4C9F-B1D0-8588267A1C82}"/>
+    <hyperlink ref="D31" r:id="rId8" xr:uid="{A901DFE1-486C-4AC2-8672-C18618945E04}"/>
+    <hyperlink ref="D29" r:id="rId9" xr:uid="{BA467D2F-0948-4A82-B49C-B8DCBA7936A0}"/>
+    <hyperlink ref="D25" r:id="rId10" xr:uid="{49178A12-AF45-4969-AC8E-49BA3EBADDA9}"/>
+    <hyperlink ref="D24" r:id="rId11" xr:uid="{537A3F3C-7C92-42A9-B8B2-F37129F7787F}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{82909F8B-3A14-4248-8CB2-384756C6E8BE}"/>
+    <hyperlink ref="D26" r:id="rId13" display="6Pcs Endstops" xr:uid="{4AEFCE09-28B7-4C24-82DE-ADAB9CAA43E1}"/>
+    <hyperlink ref="D35" r:id="rId14" xr:uid="{0ED2334F-09CF-437E-82F8-E81D86F288DC}"/>
+    <hyperlink ref="D11" r:id="rId15" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
+    <hyperlink ref="D18" r:id="rId16" display="MKS DUET WIFI Clone" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
+    <hyperlink ref="D23" r:id="rId17" xr:uid="{53A16D3E-EBE4-45B6-9E87-70111D7D2FFE}"/>
+    <hyperlink ref="F23" r:id="rId18" xr:uid="{2E01C49B-F943-468C-B222-27E06F7C15FC}"/>
+    <hyperlink ref="D16" r:id="rId19" display="Cable Loom - Bowden Path" xr:uid="{5DD23B84-72DC-46EC-A740-B82AFAD09C94}"/>
+    <hyperlink ref="D17" r:id="rId20" xr:uid="{0C6F2C79-ACBB-4C55-AC21-4895BA685D6B}"/>
+    <hyperlink ref="D19" r:id="rId21" xr:uid="{9689F2B7-24E0-4CC5-A39F-53D7E0370FC8}"/>
     <hyperlink ref="A4" r:id="rId22" xr:uid="{42E8AC4D-928E-4528-A3B8-EB12C0061FC4}"/>
     <hyperlink ref="D6" r:id="rId23" display="Bore Diameter: Bore 5mm No Teeth" xr:uid="{DC8F7F14-CA2A-4482-8C1E-5173C4B8D9AD}"/>
-    <hyperlink ref="D11" r:id="rId24" display="Color: 2GT 10MM" xr:uid="{3BB9CD36-EAAE-4CDD-91A2-546DD9AEE97B}"/>
+    <hyperlink ref="D13" r:id="rId24" display="Color: 2GT 10MM" xr:uid="{3BB9CD36-EAAE-4CDD-91A2-546DD9AEE97B}"/>
     <hyperlink ref="D32" r:id="rId25" xr:uid="{7F3B442E-F7CB-4007-B0E0-F7D6FA00B53B}"/>
     <hyperlink ref="D33" r:id="rId26" xr:uid="{EFF7A929-E8E4-4F05-A22B-23B664574CE1}"/>
-    <hyperlink ref="D19" r:id="rId27" xr:uid="{968A8156-5055-4A5F-97A2-06DF8EA0EB3D}"/>
+    <hyperlink ref="D21" r:id="rId27" xr:uid="{968A8156-5055-4A5F-97A2-06DF8EA0EB3D}"/>
     <hyperlink ref="D7" r:id="rId28" display="Bore Diameter: Bore 5mm With Teeth" xr:uid="{9AED87BC-5BEC-4990-87E4-DE18B0259F70}"/>
     <hyperlink ref="D8" r:id="rId29" display="Bore Diameter: Bore 5mm No Teeth" xr:uid="{AEF1FF18-EC10-49DF-B80B-75E1D8A2D85F}"/>
     <hyperlink ref="D9" r:id="rId30" display="Bore Diameter: Bore 5mm With Teeth" xr:uid="{5D50B8E6-99FC-422D-900D-829D1530AC87}"/>
-    <hyperlink ref="D31" r:id="rId31" xr:uid="{E2B3A9CD-7038-461B-A7D6-7375A7FBF5F4}"/>
+    <hyperlink ref="D10" r:id="rId31" xr:uid="{E2B3A9CD-7038-461B-A7D6-7375A7FBF5F4}"/>
+    <hyperlink ref="D34" r:id="rId32" xr:uid="{402BD230-D603-422A-931E-B65C09CB34DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId32"/>
-  <drawing r:id="rId33"/>
+  <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId33"/>
+  <drawing r:id="rId34"/>
   <tableParts count="1">
-    <tablePart r:id="rId34"/>
+    <tablePart r:id="rId35"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4050,14 +4079,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="152" t="s">
         <v>193</v>
       </c>
-      <c r="B1" s="153" t="s">
+      <c r="B1" s="152" t="s">
         <v>188</v>
       </c>
       <c r="C1" s="122"/>
-      <c r="D1" s="153" t="s">
+      <c r="D1" s="152" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4065,7 +4094,7 @@
       <c r="A2" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="149" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="142" t="s">
@@ -4076,10 +4105,10 @@
       <c r="A3" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="149" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="151" t="s">
+      <c r="D3" s="150" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4090,7 +4119,7 @@
       <c r="B4" s="142" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="151" t="s">
+      <c r="D4" s="150" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4101,7 +4130,7 @@
       <c r="B5" s="142" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="151" t="s">
+      <c r="D5" s="150" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4112,7 +4141,7 @@
       <c r="B6" s="142" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="151" t="s">
+      <c r="D6" s="150" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4120,21 +4149,21 @@
       <c r="A7" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="B7" s="151" t="s">
+      <c r="B7" s="150" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="150" t="s">
+      <c r="D7" s="149" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="149" t="s">
+      <c r="A8" s="148" t="s">
         <v>202</v>
       </c>
       <c r="B8" s="143" t="s">
         <v>192</v>
       </c>
-      <c r="D8" s="152" t="s">
+      <c r="D8" s="151" t="s">
         <v>191</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bom update for 10mm belt
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-Baby BOM.xlsx
+++ b/Document Library/Bill Of Materials/V-Baby BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-Baby CoreXY/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2480" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8CB3C518-702F-4E34-9682-27010B221D45}"/>
+  <xr:revisionPtr revIDLastSave="2531" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E899A878-221C-42F9-8DDE-18B5C6A2148C}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="252">
   <si>
     <t>Exstrusions</t>
   </si>
@@ -574,12 +574,6 @@
     <t>Thoothed Idler for 10mm belt</t>
   </si>
   <si>
-    <t>Belt Timing Belt 6mm</t>
-  </si>
-  <si>
-    <t>Belt Timing Belt 10mm</t>
-  </si>
-  <si>
     <t>4 meter</t>
   </si>
   <si>
@@ -598,9 +592,6 @@
     <t>No cuts - No tapps</t>
   </si>
   <si>
-    <t>Z 3:1 GT2 Gear Pulleys</t>
-  </si>
-  <si>
     <t>WORM GEAR</t>
   </si>
   <si>
@@ -673,12 +664,6 @@
     <t>10mm Belt Idler Thoothed</t>
   </si>
   <si>
-    <t>4M Color: 2GT 6MM</t>
-  </si>
-  <si>
-    <t>2M Color: 2GT 10MM</t>
-  </si>
-  <si>
     <t>Size: Black 1M</t>
   </si>
   <si>
@@ -691,9 +676,6 @@
     <t>Fan for Cabinet cooling</t>
   </si>
   <si>
-    <t>Fan Part Cooling</t>
-  </si>
-  <si>
     <t>Stepper motor 1.8 Amp</t>
   </si>
   <si>
@@ -733,9 +715,6 @@
     <t>5mm Length: 35mm 6PC</t>
   </si>
   <si>
-    <t>Belt Motor Pulley GT2</t>
-  </si>
-  <si>
     <t>Belt Idler Bearing shafts</t>
   </si>
   <si>
@@ -748,9 +727,6 @@
     <t>Bolt for the Gear Pulleys</t>
   </si>
   <si>
-    <t>M5 Length: 60mm</t>
-  </si>
-  <si>
     <t>Size: W 11mm without t</t>
   </si>
   <si>
@@ -760,7 +736,61 @@
     <t>Size: W 7mm with t</t>
   </si>
   <si>
-    <t>pulley</t>
+    <t>Z 3:1 GT2 Gear</t>
+  </si>
+  <si>
+    <t>Dia 5mm Length: 60mm</t>
+  </si>
+  <si>
+    <t>10mm Belt Idler Smooth</t>
+  </si>
+  <si>
+    <t>6mm Belt Motor Pulley</t>
+  </si>
+  <si>
+    <t>10mm Timing Belt</t>
+  </si>
+  <si>
+    <t>6mm Timing Belt</t>
+  </si>
+  <si>
+    <t>10mm Belt Z Gear Pulley</t>
+  </si>
+  <si>
+    <t>Pulley for the Belted Z Gear</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Fan For Part Cooling</t>
+  </si>
+  <si>
+    <t>Size: For 10mm 1 pcs</t>
+  </si>
+  <si>
+    <t>Size: 4M-6MM-2GT</t>
+  </si>
+  <si>
+    <t>Size: 2M Color: 2GT 10MM</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1380,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1569,16 +1599,25 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="40 % – uthevingsfarge 6" xfId="4" builtinId="51"/>
-    <cellStyle name="God" xfId="1" builtinId="26"/>
-    <cellStyle name="Hyperkobling" xfId="3" builtinId="8"/>
+    <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nøytral" xfId="5" builtinId="28"/>
-    <cellStyle name="Uthevingsfarge1" xfId="2" builtinId="29"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="8">
     <dxf>
       <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1593,40 +1632,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
@@ -1644,23 +1649,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1673,23 +1661,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1724,38 +1695,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1768,72 +1707,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2159,25 +2032,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1070DF90-74AC-4245-AA46-2FAD63F74767}" name="Table1" displayName="Table1" ref="A6:G35" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:G35">
-    <sortCondition ref="A6:A35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1070DF90-74AC-4245-AA46-2FAD63F74767}" name="Table1" displayName="Table1" ref="A6:G37" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G37">
+    <sortCondition ref="A7:A37"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AB8C8187-911D-4248-8608-1F70796FF7C8}" name="Column1" headerRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{129F7AE4-0D03-4AA3-A2BF-5181AA27AF31}" name="Column2" headerRowDxfId="10" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{34C25536-CCA4-454C-9FCE-0168DD2CC6CC}" name="Column3" headerRowDxfId="8" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{2ABF818D-0A23-4468-A061-EB5B1AC04237}" name="Column4" headerRowDxfId="6" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{3DD38B84-FE10-46EA-8CEE-8542F56DCDD7}" name="Column5" headerRowDxfId="4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{E4DF9CF3-4A3D-433E-9BD0-F94DDCA192BB}" name="Column6" headerRowDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{4866A326-BBBA-4B58-BFBD-4D095130E124}" name="Column7" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AB8C8187-911D-4248-8608-1F70796FF7C8}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{129F7AE4-0D03-4AA3-A2BF-5181AA27AF31}" name="Column2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{34C25536-CCA4-454C-9FCE-0168DD2CC6CC}" name="Column3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2ABF818D-0A23-4468-A061-EB5B1AC04237}" name="Column4" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{3DD38B84-FE10-46EA-8CEE-8542F56DCDD7}" name="Column5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E4DF9CF3-4A3D-433E-9BD0-F94DDCA192BB}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{4866A326-BBBA-4B58-BFBD-4D095130E124}" name="Column7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2503,7 +2376,7 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.54296875" customWidth="1"/>
     <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
@@ -2705,7 +2578,7 @@
       <c r="F15" s="157"/>
       <c r="G15" s="40"/>
       <c r="H15" s="49" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="59"/>
@@ -2728,7 +2601,7 @@
       <c r="F16" s="157"/>
       <c r="G16" s="40"/>
       <c r="H16" s="51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I16" s="60" t="s">
         <v>120</v>
@@ -2871,8 +2744,8 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="146">
-        <f>'Component Part List'!$E$36</f>
-        <v>509.5</v>
+        <f>'Component Part List'!$E$38</f>
+        <v>515.5</v>
       </c>
       <c r="G25" s="41"/>
       <c r="H25" s="26" t="s">
@@ -2880,8 +2753,8 @@
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="146">
-        <f>'Component Part List'!$E$36</f>
-        <v>509.5</v>
+        <f>'Component Part List'!$E$38</f>
+        <v>515.5</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -2935,7 +2808,7 @@
       <c r="E28" s="38"/>
       <c r="F28" s="34">
         <f>SUM(F24:F27)</f>
-        <v>869.5</v>
+        <v>875.5</v>
       </c>
       <c r="G28" s="41"/>
       <c r="H28" s="52" t="s">
@@ -2944,7 +2817,7 @@
       <c r="I28" s="53"/>
       <c r="J28" s="54">
         <f>SUM(J24:J27)</f>
-        <v>748.1</v>
+        <v>754.1</v>
       </c>
     </row>
   </sheetData>
@@ -2970,7 +2843,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="3" max="3" width="6.26953125" style="72" customWidth="1"/>
@@ -3333,13 +3206,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
@@ -3416,170 +3287,174 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="158" t="s">
         <v>241</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="91">
-        <v>4</v>
-      </c>
-      <c r="D6" s="105" t="s">
-        <v>238</v>
-      </c>
-      <c r="E6" s="102">
-        <v>16</v>
-      </c>
-      <c r="F6" s="92"/>
-      <c r="G6" s="153"/>
+      <c r="B6" s="87" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" s="159" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="160" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="160" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" s="160" t="s">
+        <v>246</v>
+      </c>
+      <c r="G6" s="160" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="7" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C7" s="91">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" s="105" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E7" s="102">
-        <v>10</v>
-      </c>
-      <c r="F7" s="96"/>
-      <c r="G7" s="103"/>
+        <v>16</v>
+      </c>
+      <c r="F7" s="92"/>
+      <c r="G7" s="153"/>
     </row>
     <row r="8" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C8" s="91">
         <v>2</v>
       </c>
       <c r="D8" s="105" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E8" s="102">
         <v>10</v>
       </c>
-      <c r="F8" s="92"/>
-      <c r="G8" s="102"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="103"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>177</v>
+        <v>240</v>
       </c>
       <c r="C9" s="91">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D9" s="105" t="s">
-        <v>240</v>
-      </c>
-      <c r="E9" s="102">
-        <v>28</v>
-      </c>
-      <c r="F9" s="96"/>
+        <v>249</v>
+      </c>
+      <c r="E9" s="103">
+        <v>5</v>
+      </c>
+      <c r="F9" s="15"/>
       <c r="G9" s="103"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="C10" s="91" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" s="154" t="s">
-        <v>231</v>
+        <v>180</v>
+      </c>
+      <c r="D10" s="105" t="s">
+        <v>251</v>
       </c>
       <c r="E10" s="103">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="103"/>
     </row>
     <row r="11" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>150</v>
+        <v>206</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="C11" s="91">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="D11" s="105" t="s">
-        <v>204</v>
+        <v>230</v>
       </c>
       <c r="E11" s="102">
-        <v>15</v>
-      </c>
-      <c r="F11" s="96"/>
-      <c r="G11" s="103"/>
+        <v>10</v>
+      </c>
+      <c r="F11" s="92"/>
+      <c r="G11" s="102"/>
     </row>
     <row r="12" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="91">
+        <v>6</v>
+      </c>
+      <c r="D12" s="105" t="s">
         <v>232</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="91">
-        <v>2</v>
-      </c>
-      <c r="D12" s="105" t="s">
-        <v>208</v>
-      </c>
-      <c r="E12" s="103">
-        <v>11</v>
-      </c>
-      <c r="F12" s="15"/>
+      <c r="E12" s="102">
+        <v>28</v>
+      </c>
+      <c r="F12" s="96"/>
       <c r="G12" s="103"/>
     </row>
     <row r="13" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="C13" s="91" t="s">
-        <v>182</v>
+        <v>68</v>
+      </c>
+      <c r="C13" s="91">
+        <v>2</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E13" s="103">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="103"/>
     </row>
     <row r="14" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="91" t="s">
         <v>179</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" s="91" t="s">
-        <v>181</v>
-      </c>
       <c r="D14" s="105" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="E14" s="103">
         <v>19</v>
@@ -3589,474 +3464,513 @@
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>60</v>
+        <v>226</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="91">
-        <v>1</v>
-      </c>
-      <c r="D15" s="105" t="s">
-        <v>214</v>
+        <v>224</v>
+      </c>
+      <c r="C15" s="91" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="154" t="s">
+        <v>225</v>
       </c>
       <c r="E15" s="103">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="103"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
-        <v>161</v>
+      <c r="A16" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C16" s="91">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>160</v>
-      </c>
-      <c r="E16" s="103">
-        <v>2.5</v>
-      </c>
-      <c r="F16" s="15"/>
+        <v>201</v>
+      </c>
+      <c r="E16" s="102">
+        <v>15</v>
+      </c>
+      <c r="F16" s="96"/>
       <c r="G16" s="103"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="C17" s="91">
         <v>1</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="E17" s="103">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="103"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>42</v>
+      <c r="A18" s="14" t="s">
+        <v>161</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="C18" s="91">
         <v>1</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="E18" s="103">
-        <v>60</v>
-      </c>
-      <c r="F18" s="96"/>
+        <v>2.5</v>
+      </c>
+      <c r="F18" s="15"/>
       <c r="G18" s="103"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>59</v>
+        <v>165</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C19" s="91">
         <v>1</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E19" s="103">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="103"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>217</v>
+        <v>42</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="C20" s="91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="E20" s="103">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F20" s="96"/>
       <c r="G20" s="103"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>216</v>
+        <v>59</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="C21" s="91">
         <v>1</v>
       </c>
       <c r="D21" s="105" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="E21" s="103">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="103"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C22" s="91">
         <v>2</v>
       </c>
       <c r="D22" s="105" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E22" s="103">
         <v>10</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="96"/>
       <c r="G22" s="103"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>155</v>
+        <v>44</v>
       </c>
       <c r="C23" s="91">
         <v>1</v>
       </c>
       <c r="D23" s="105" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="E23" s="103">
-        <v>30</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="G23" s="103">
-        <v>16</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="103"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>167</v>
+        <v>248</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="C24" s="91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="105" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="E24" s="103">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="103"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>220</v>
+        <v>152</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="C25" s="91" t="s">
-        <v>222</v>
+        <v>155</v>
+      </c>
+      <c r="C25" s="91">
+        <v>1</v>
       </c>
       <c r="D25" s="105" t="s">
-        <v>221</v>
+        <v>156</v>
       </c>
       <c r="E25" s="103">
         <v>30</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="103"/>
+      <c r="F25" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="103">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="108" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="91" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="91">
+        <v>1</v>
+      </c>
+      <c r="D26" s="105" t="s">
         <v>223</v>
       </c>
-      <c r="D26" s="105" t="s">
-        <v>169</v>
-      </c>
       <c r="E26" s="103">
-        <v>4</v>
-      </c>
-      <c r="F26" s="96"/>
+        <v>73</v>
+      </c>
+      <c r="F26" s="15"/>
       <c r="G26" s="103"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>65</v>
+        <v>214</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="91">
-        <v>1</v>
+        <v>213</v>
+      </c>
+      <c r="C27" s="91" t="s">
+        <v>216</v>
       </c>
       <c r="D27" s="105" t="s">
-        <v>67</v>
+        <v>215</v>
       </c>
       <c r="E27" s="103">
-        <v>8.5</v>
+        <v>30</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="103"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="91">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="B28" s="108" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="91" t="s">
+        <v>217</v>
       </c>
       <c r="D28" s="105" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="E28" s="103">
-        <v>20</v>
-      </c>
-      <c r="F28" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="F28" s="96"/>
       <c r="G28" s="103"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C29" s="91">
         <v>1</v>
       </c>
       <c r="D29" s="105" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E29" s="103">
-        <v>2</v>
-      </c>
-      <c r="F29" s="100"/>
+        <v>8.5</v>
+      </c>
+      <c r="F29" s="15"/>
       <c r="G29" s="103"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C30" s="91">
         <v>1</v>
       </c>
       <c r="D30" s="105" t="s">
-        <v>224</v>
+        <v>64</v>
       </c>
       <c r="E30" s="103">
-        <v>40</v>
-      </c>
-      <c r="F30" s="100"/>
+        <v>20</v>
+      </c>
+      <c r="F30" s="15"/>
       <c r="G30" s="103"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C31" s="91">
         <v>1</v>
       </c>
       <c r="D31" s="105" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E31" s="103">
-        <v>3.5</v>
-      </c>
-      <c r="F31" s="155"/>
+        <v>2</v>
+      </c>
+      <c r="F31" s="100"/>
       <c r="G31" s="103"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>187</v>
+        <v>51</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>203</v>
+        <v>52</v>
       </c>
       <c r="C32" s="91">
         <v>1</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>225</v>
+      <c r="D32" s="105" t="s">
+        <v>218</v>
       </c>
       <c r="E32" s="103">
-        <v>8.5</v>
-      </c>
-      <c r="F32" s="15"/>
+        <v>40</v>
+      </c>
+      <c r="F32" s="100"/>
       <c r="G32" s="103"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>234</v>
+        <v>53</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="C33" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D33" s="147" t="s">
-        <v>228</v>
+        <v>54</v>
+      </c>
+      <c r="C33" s="91">
+        <v>1</v>
+      </c>
+      <c r="D33" s="105" t="s">
+        <v>55</v>
       </c>
       <c r="E33" s="103">
-        <v>19</v>
-      </c>
-      <c r="F33" s="15"/>
+        <v>3.5</v>
+      </c>
+      <c r="F33" s="155"/>
       <c r="G33" s="103"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
       <c r="C34" s="91">
         <v>1</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="E34" s="103">
-        <v>6</v>
+        <v>8.5</v>
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="103"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="91" t="s">
+        <v>220</v>
+      </c>
+      <c r="D35" s="147" t="s">
+        <v>222</v>
+      </c>
+      <c r="E35" s="103">
+        <v>19</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="103"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C36" s="91">
+        <v>1</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="E36" s="103">
+        <v>6</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="103"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="109" t="s">
+      <c r="B37" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="107">
+      <c r="C37" s="107">
         <v>1</v>
       </c>
-      <c r="D35" s="106" t="s">
+      <c r="D37" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="E35" s="104">
+      <c r="E37" s="104">
         <v>14</v>
       </c>
-      <c r="F35" s="101"/>
-      <c r="G35" s="104"/>
-    </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="93" t="s">
+      <c r="F37" s="101"/>
+      <c r="G37" s="104"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="94"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
-      <c r="E36" s="95">
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="95">
         <f>SUBTOTAL(109,Table1[[#All],[Column5]])</f>
-        <v>509.5</v>
-      </c>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-    </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="124" t="s">
+        <v>515.5</v>
+      </c>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="124" t="s">
         <v>174</v>
       </c>
-      <c r="B37" s="125"/>
-      <c r="C37" s="125"/>
-      <c r="D37" s="125"/>
-      <c r="E37" s="126">
-        <f>E4+E36</f>
-        <v>843.5</v>
+      <c r="B39" s="125"/>
+      <c r="C39" s="125"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="126">
+        <f>E4+E38</f>
+        <v>849.5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D30" r:id="rId1" display="220V/110V" xr:uid="{3773511A-F3AF-4897-B5BB-16FB39A0B508}"/>
-    <hyperlink ref="D20" r:id="rId2" xr:uid="{AFC120EB-E75F-4BB8-BC6D-4AA9408DD14D}"/>
-    <hyperlink ref="D28" r:id="rId3" display="Link" xr:uid="{401DDADA-DB79-4416-96CF-3B1D6329769B}"/>
-    <hyperlink ref="D22" r:id="rId4" display="24V Dual Ball" xr:uid="{98BCAD8D-1DD9-49E5-B60D-FB8A39108E71}"/>
-    <hyperlink ref="D14" r:id="rId5" xr:uid="{9F0DE403-B0EC-4933-928F-2806FBCF603A}"/>
-    <hyperlink ref="D27" r:id="rId6" display="Link" xr:uid="{45531F32-6B6C-44D5-9B2A-FB1F259BC9F9}"/>
-    <hyperlink ref="D12" r:id="rId7" xr:uid="{43C03DCA-7867-4C9F-B1D0-8588267A1C82}"/>
-    <hyperlink ref="D31" r:id="rId8" xr:uid="{A901DFE1-486C-4AC2-8672-C18618945E04}"/>
-    <hyperlink ref="D29" r:id="rId9" xr:uid="{BA467D2F-0948-4A82-B49C-B8DCBA7936A0}"/>
-    <hyperlink ref="D25" r:id="rId10" xr:uid="{49178A12-AF45-4969-AC8E-49BA3EBADDA9}"/>
-    <hyperlink ref="D24" r:id="rId11" xr:uid="{537A3F3C-7C92-42A9-B8B2-F37129F7787F}"/>
-    <hyperlink ref="D15" r:id="rId12" xr:uid="{82909F8B-3A14-4248-8CB2-384756C6E8BE}"/>
-    <hyperlink ref="D26" r:id="rId13" display="6Pcs Endstops" xr:uid="{4AEFCE09-28B7-4C24-82DE-ADAB9CAA43E1}"/>
-    <hyperlink ref="D35" r:id="rId14" xr:uid="{0ED2334F-09CF-437E-82F8-E81D86F288DC}"/>
-    <hyperlink ref="D11" r:id="rId15" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
-    <hyperlink ref="D18" r:id="rId16" display="MKS DUET WIFI Clone" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
-    <hyperlink ref="D23" r:id="rId17" xr:uid="{53A16D3E-EBE4-45B6-9E87-70111D7D2FFE}"/>
-    <hyperlink ref="F23" r:id="rId18" xr:uid="{2E01C49B-F943-468C-B222-27E06F7C15FC}"/>
-    <hyperlink ref="D16" r:id="rId19" display="Cable Loom - Bowden Path" xr:uid="{5DD23B84-72DC-46EC-A740-B82AFAD09C94}"/>
-    <hyperlink ref="D17" r:id="rId20" xr:uid="{0C6F2C79-ACBB-4C55-AC21-4895BA685D6B}"/>
-    <hyperlink ref="D19" r:id="rId21" xr:uid="{9689F2B7-24E0-4CC5-A39F-53D7E0370FC8}"/>
+    <hyperlink ref="D32" r:id="rId1" display="220V/110V" xr:uid="{3773511A-F3AF-4897-B5BB-16FB39A0B508}"/>
+    <hyperlink ref="D22" r:id="rId2" xr:uid="{AFC120EB-E75F-4BB8-BC6D-4AA9408DD14D}"/>
+    <hyperlink ref="D30" r:id="rId3" display="Link" xr:uid="{401DDADA-DB79-4416-96CF-3B1D6329769B}"/>
+    <hyperlink ref="D24" r:id="rId4" display="24V Dual Ball" xr:uid="{98BCAD8D-1DD9-49E5-B60D-FB8A39108E71}"/>
+    <hyperlink ref="D14" r:id="rId5" display="4M Color: 2GT 6MM" xr:uid="{9F0DE403-B0EC-4933-928F-2806FBCF603A}"/>
+    <hyperlink ref="D29" r:id="rId6" display="Link" xr:uid="{45531F32-6B6C-44D5-9B2A-FB1F259BC9F9}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{43C03DCA-7867-4C9F-B1D0-8588267A1C82}"/>
+    <hyperlink ref="D33" r:id="rId8" xr:uid="{A901DFE1-486C-4AC2-8672-C18618945E04}"/>
+    <hyperlink ref="D31" r:id="rId9" xr:uid="{BA467D2F-0948-4A82-B49C-B8DCBA7936A0}"/>
+    <hyperlink ref="D27" r:id="rId10" xr:uid="{49178A12-AF45-4969-AC8E-49BA3EBADDA9}"/>
+    <hyperlink ref="D26" r:id="rId11" xr:uid="{537A3F3C-7C92-42A9-B8B2-F37129F7787F}"/>
+    <hyperlink ref="D17" r:id="rId12" xr:uid="{82909F8B-3A14-4248-8CB2-384756C6E8BE}"/>
+    <hyperlink ref="D28" r:id="rId13" display="6Pcs Endstops" xr:uid="{4AEFCE09-28B7-4C24-82DE-ADAB9CAA43E1}"/>
+    <hyperlink ref="D37" r:id="rId14" xr:uid="{0ED2334F-09CF-437E-82F8-E81D86F288DC}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{A333F16C-7F8A-421A-B64A-B04B701B747A}"/>
+    <hyperlink ref="D20" r:id="rId16" display="MKS DUET WIFI Clone" xr:uid="{F52EB8DF-670A-4145-90A1-8A8DF8B4B7B2}"/>
+    <hyperlink ref="D25" r:id="rId17" xr:uid="{53A16D3E-EBE4-45B6-9E87-70111D7D2FFE}"/>
+    <hyperlink ref="F25" r:id="rId18" xr:uid="{2E01C49B-F943-468C-B222-27E06F7C15FC}"/>
+    <hyperlink ref="D18" r:id="rId19" display="Cable Loom - Bowden Path" xr:uid="{5DD23B84-72DC-46EC-A740-B82AFAD09C94}"/>
+    <hyperlink ref="D19" r:id="rId20" xr:uid="{0C6F2C79-ACBB-4C55-AC21-4895BA685D6B}"/>
+    <hyperlink ref="D21" r:id="rId21" xr:uid="{9689F2B7-24E0-4CC5-A39F-53D7E0370FC8}"/>
     <hyperlink ref="A4" r:id="rId22" xr:uid="{42E8AC4D-928E-4528-A3B8-EB12C0061FC4}"/>
-    <hyperlink ref="D6" r:id="rId23" display="Bore 5mm No Teeth:For belt width 10mm" xr:uid="{DC8F7F14-CA2A-4482-8C1E-5173C4B8D9AD}"/>
-    <hyperlink ref="D13" r:id="rId24" display="Color: 2GT 10MM" xr:uid="{3BB9CD36-EAAE-4CDD-91A2-546DD9AEE97B}"/>
-    <hyperlink ref="D32" r:id="rId25" xr:uid="{7F3B442E-F7CB-4007-B0E0-F7D6FA00B53B}"/>
-    <hyperlink ref="D33" r:id="rId26" xr:uid="{EFF7A929-E8E4-4F05-A22B-23B664574CE1}"/>
-    <hyperlink ref="D21" r:id="rId27" xr:uid="{968A8156-5055-4A5F-97A2-06DF8EA0EB3D}"/>
-    <hyperlink ref="D7" r:id="rId28" display="Bore 5mm With Teeth:For belt width 10mm" xr:uid="{9AED87BC-5BEC-4990-87E4-DE18B0259F70}"/>
-    <hyperlink ref="D8" r:id="rId29" display="Bore 5mm No Teeth:For belt width 6mm" xr:uid="{AEF1FF18-EC10-49DF-B80B-75E1D8A2D85F}"/>
-    <hyperlink ref="D9" r:id="rId30" display="Bore 5mm With Teeth:For belt width 6mm" xr:uid="{5D50B8E6-99FC-422D-900D-829D1530AC87}"/>
-    <hyperlink ref="D10" r:id="rId31" xr:uid="{E2B3A9CD-7038-461B-A7D6-7375A7FBF5F4}"/>
-    <hyperlink ref="D34" r:id="rId32" display="M5 Length: 55mm" xr:uid="{402BD230-D603-422A-931E-B65C09CB34DA}"/>
+    <hyperlink ref="D7" r:id="rId23" display="Bore 5mm No Teeth:For belt width 10mm" xr:uid="{DC8F7F14-CA2A-4482-8C1E-5173C4B8D9AD}"/>
+    <hyperlink ref="D10" r:id="rId24" display="Color: 2GT 10MM" xr:uid="{3BB9CD36-EAAE-4CDD-91A2-546DD9AEE97B}"/>
+    <hyperlink ref="D34" r:id="rId25" xr:uid="{7F3B442E-F7CB-4007-B0E0-F7D6FA00B53B}"/>
+    <hyperlink ref="D35" r:id="rId26" xr:uid="{EFF7A929-E8E4-4F05-A22B-23B664574CE1}"/>
+    <hyperlink ref="D23" r:id="rId27" xr:uid="{968A8156-5055-4A5F-97A2-06DF8EA0EB3D}"/>
+    <hyperlink ref="D8" r:id="rId28" display="Bore 5mm With Teeth:For belt width 10mm" xr:uid="{9AED87BC-5BEC-4990-87E4-DE18B0259F70}"/>
+    <hyperlink ref="D11" r:id="rId29" display="Bore 5mm No Teeth:For belt width 6mm" xr:uid="{AEF1FF18-EC10-49DF-B80B-75E1D8A2D85F}"/>
+    <hyperlink ref="D12" r:id="rId30" display="Bore 5mm With Teeth:For belt width 6mm" xr:uid="{5D50B8E6-99FC-422D-900D-829D1530AC87}"/>
+    <hyperlink ref="D15" r:id="rId31" xr:uid="{E2B3A9CD-7038-461B-A7D6-7375A7FBF5F4}"/>
+    <hyperlink ref="D36" r:id="rId32" display="M5 Length: 55mm" xr:uid="{402BD230-D603-422A-931E-B65C09CB34DA}"/>
+    <hyperlink ref="D9" r:id="rId33" display="For 10mm 1 pcs" xr:uid="{7BA0A6EE-6125-4655-AC0E-C61D1887FEFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId33"/>
-  <drawing r:id="rId34"/>
+  <pageSetup paperSize="9" scale="86" orientation="landscape" r:id="rId34"/>
+  <drawing r:id="rId35"/>
   <tableParts count="1">
-    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId36"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4069,7 +3983,7 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
@@ -4079,91 +3993,91 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="152" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B1" s="152" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C1" s="122"/>
       <c r="D1" s="152" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B2" s="149" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D2" s="142" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B3" s="149" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D3" s="150" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B4" s="142" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="150" t="s">
         <v>192</v>
-      </c>
-      <c r="D4" s="150" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B5" s="142" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D5" s="150" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B6" s="142" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="150" t="s">
         <v>192</v>
-      </c>
-      <c r="D6" s="150" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B7" s="150" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D7" s="149" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="148" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B8" s="143" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D8" s="151" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -4177,7 +4091,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
@@ -4756,7 +4670,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
updated belt length for the 300 size option. buy 4m not 2
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-Baby BOM.xlsx
+++ b/Document Library/Bill Of Materials/V-Baby BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-Baby CoreXY/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2533" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91E6F13B-7B6A-43FA-80DD-652DB1CC48FB}"/>
+  <xr:revisionPtr revIDLastSave="2536" documentId="11_2E462098BBA7632759C38D02185E4833A2B67484" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7FA8670-BA6E-4E24-9F01-71D410423B88}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpenBuild Part List" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="252">
   <si>
     <t>Exstrusions</t>
   </si>
@@ -575,9 +575,6 @@
   </si>
   <si>
     <t>4 meter</t>
-  </si>
-  <si>
-    <t>2 meter</t>
   </si>
   <si>
     <t>2GT Timing Belt 10W 2 Meter</t>
@@ -2379,20 +2376,20 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" customWidth="1"/>
-    <col min="7" max="7" width="4.26953125" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
@@ -2420,7 +2417,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2434,7 +2431,7 @@
       <c r="I8" s="42"/>
       <c r="J8" s="58"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>7</v>
       </c>
@@ -2457,7 +2454,7 @@
       <c r="I9" s="15"/>
       <c r="J9" s="59"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>10</v>
       </c>
@@ -2480,7 +2477,7 @@
       <c r="I10" s="42"/>
       <c r="J10" s="58"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>13</v>
       </c>
@@ -2503,7 +2500,7 @@
       <c r="I11" s="15"/>
       <c r="J11" s="59"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>16</v>
       </c>
@@ -2526,7 +2523,7 @@
       <c r="I12" s="42"/>
       <c r="J12" s="58"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2538,7 +2535,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="59"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
         <v>18</v>
       </c>
@@ -2561,7 +2558,7 @@
       <c r="I14" s="42"/>
       <c r="J14" s="58"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
         <v>21</v>
       </c>
@@ -2581,12 +2578,12 @@
       <c r="F15" s="160"/>
       <c r="G15" s="40"/>
       <c r="H15" s="49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="59"/>
     </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>24</v>
       </c>
@@ -2604,7 +2601,7 @@
       <c r="F16" s="160"/>
       <c r="G16" s="40"/>
       <c r="H16" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I16" s="60" t="s">
         <v>120</v>
@@ -2613,7 +2610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2629,7 +2626,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
         <v>28</v>
       </c>
@@ -2655,7 +2652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2667,7 +2664,7 @@
       <c r="I19" s="61"/>
       <c r="J19" s="59"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="48" t="s">
         <v>31</v>
       </c>
@@ -2693,7 +2690,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
@@ -2712,11 +2709,11 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>36</v>
       </c>
@@ -2738,7 +2735,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>37</v>
       </c>
@@ -2748,7 +2745,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="146">
         <f>'Component Part List'!$E$38</f>
-        <v>515.5</v>
+        <v>523.5</v>
       </c>
       <c r="G25" s="41"/>
       <c r="H25" s="26" t="s">
@@ -2757,10 +2754,10 @@
       <c r="I25" s="6"/>
       <c r="J25" s="146">
         <f>'Component Part List'!$E$38</f>
-        <v>515.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+        <v>523.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>38</v>
       </c>
@@ -2780,7 +2777,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
         <v>40</v>
       </c>
@@ -2801,7 +2798,7 @@
         <v>80.600000000000009</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
         <v>119</v>
       </c>
@@ -2811,7 +2808,7 @@
       <c r="E28" s="38"/>
       <c r="F28" s="34">
         <f>SUM(F24:F27)</f>
-        <v>875.5</v>
+        <v>883.5</v>
       </c>
       <c r="G28" s="41"/>
       <c r="H28" s="52" t="s">
@@ -2820,7 +2817,7 @@
       <c r="I28" s="53"/>
       <c r="J28" s="54">
         <f>SUM(J24:J27)</f>
-        <v>754.1</v>
+        <v>762.1</v>
       </c>
     </row>
   </sheetData>
@@ -2846,14 +2843,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" style="72" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="72" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A6" s="74" t="s">
         <v>125</v>
       </c>
@@ -2864,7 +2861,7 @@
       <c r="F6" s="75"/>
       <c r="G6" s="77"/>
     </row>
-    <row r="7" spans="1:7" s="73" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="128" t="s">
         <v>126</v>
       </c>
@@ -2881,7 +2878,7 @@
       </c>
       <c r="G7" s="129"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
         <v>140</v>
       </c>
@@ -2902,7 +2899,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
         <v>141</v>
       </c>
@@ -2927,7 +2924,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="78" t="s">
         <v>142</v>
       </c>
@@ -2948,7 +2945,7 @@
       </c>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="78" t="s">
         <v>18</v>
       </c>
@@ -2969,7 +2966,7 @@
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="78" t="s">
         <v>21</v>
       </c>
@@ -2990,7 +2987,7 @@
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="84" t="s">
         <v>16</v>
       </c>
@@ -3011,7 +3008,7 @@
       </c>
       <c r="G13" s="85"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="78"/>
       <c r="B14" s="6"/>
       <c r="C14" s="79"/>
@@ -3020,7 +3017,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" s="73" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="80" t="s">
         <v>133</v>
       </c>
@@ -3031,7 +3028,7 @@
       <c r="F15" s="81"/>
       <c r="G15" s="83"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="78" t="s">
         <v>132</v>
       </c>
@@ -3042,7 +3039,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="140" t="s">
         <v>134</v>
       </c>
@@ -3059,7 +3056,7 @@
       </c>
       <c r="G17" s="77"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="78" t="s">
         <v>140</v>
       </c>
@@ -3079,7 +3076,7 @@
       </c>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="78" t="s">
         <v>141</v>
       </c>
@@ -3101,7 +3098,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="78" t="s">
         <v>142</v>
       </c>
@@ -3121,7 +3118,7 @@
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="78" t="s">
         <v>18</v>
       </c>
@@ -3137,7 +3134,7 @@
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
         <v>21</v>
       </c>
@@ -3153,7 +3150,7 @@
       </c>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="84" t="s">
         <v>16</v>
       </c>
@@ -3169,7 +3166,7 @@
       </c>
       <c r="G23" s="85"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="79"/>
@@ -3178,17 +3175,17 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>139</v>
       </c>
@@ -3211,22 +3208,20 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="4" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.26953125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="110"/>
       <c r="B1" s="75"/>
       <c r="C1" s="75"/>
@@ -3235,7 +3230,7 @@
       <c r="F1" s="112"/>
       <c r="G1" s="113"/>
     </row>
-    <row r="2" spans="1:7" ht="27" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="27.75" x14ac:dyDescent="0.5">
       <c r="A2" s="114"/>
       <c r="B2" s="90"/>
       <c r="C2" s="97"/>
@@ -3246,7 +3241,7 @@
       <c r="F2" s="89"/>
       <c r="G2" s="115"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="78"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3255,7 +3250,7 @@
       <c r="F3" s="86"/>
       <c r="G3" s="116"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="120" t="s">
         <v>172</v>
       </c>
@@ -3269,7 +3264,7 @@
       </c>
       <c r="G4" s="117"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="118" t="s">
         <v>1</v>
       </c>
@@ -3292,32 +3287,32 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="87" t="s">
         <v>241</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="C6" s="157" t="s">
         <v>242</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="D6" s="158" t="s">
         <v>243</v>
       </c>
-      <c r="D6" s="158" t="s">
+      <c r="E6" s="158" t="s">
         <v>244</v>
       </c>
-      <c r="E6" s="158" t="s">
+      <c r="F6" s="158" t="s">
         <v>245</v>
       </c>
-      <c r="F6" s="158" t="s">
+      <c r="G6" s="158" t="s">
         <v>246</v>
       </c>
-      <c r="G6" s="158" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>176</v>
@@ -3326,7 +3321,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="105" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E7" s="102">
         <v>16</v>
@@ -3334,9 +3329,9 @@
       <c r="F7" s="92"/>
       <c r="G7" s="153"/>
     </row>
-    <row r="8" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>178</v>
@@ -3345,7 +3340,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="105" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E8" s="102">
         <v>10</v>
@@ -3353,18 +3348,18 @@
       <c r="F8" s="96"/>
       <c r="G8" s="103"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>239</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>240</v>
       </c>
       <c r="C9" s="91">
         <v>1</v>
       </c>
       <c r="D9" s="105" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E9" s="103">
         <v>5</v>
@@ -3372,28 +3367,28 @@
       <c r="F9" s="15"/>
       <c r="G9" s="103"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" s="91" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D10" s="105" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E10" s="103">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="103"/>
     </row>
-    <row r="11" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>175</v>
@@ -3402,7 +3397,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="105" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E11" s="102">
         <v>10</v>
@@ -3410,9 +3405,9 @@
       <c r="F11" s="92"/>
       <c r="G11" s="102"/>
     </row>
-    <row r="12" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>177</v>
@@ -3421,7 +3416,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="105" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E12" s="102">
         <v>28</v>
@@ -3429,9 +3424,9 @@
       <c r="F12" s="96"/>
       <c r="G12" s="103"/>
     </row>
-    <row r="13" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>68</v>
@@ -3440,7 +3435,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E13" s="103">
         <v>11</v>
@@ -3448,18 +3443,18 @@
       <c r="F13" s="15"/>
       <c r="G13" s="103"/>
     </row>
-    <row r="14" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14" s="91" t="s">
         <v>179</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E14" s="103">
         <v>19</v>
@@ -3467,18 +3462,18 @@
       <c r="F14" s="15"/>
       <c r="G14" s="103"/>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B15" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="C15" s="91" t="s">
+        <v>216</v>
+      </c>
+      <c r="D15" s="154" t="s">
         <v>224</v>
-      </c>
-      <c r="C15" s="91" t="s">
-        <v>217</v>
-      </c>
-      <c r="D15" s="154" t="s">
-        <v>225</v>
       </c>
       <c r="E15" s="103">
         <v>3</v>
@@ -3486,7 +3481,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="103"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>150</v>
       </c>
@@ -3497,7 +3492,7 @@
         <v>80</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E16" s="102">
         <v>15</v>
@@ -3505,7 +3500,7 @@
       <c r="F16" s="96"/>
       <c r="G16" s="103"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>60</v>
       </c>
@@ -3516,7 +3511,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E17" s="103">
         <v>2.5</v>
@@ -3524,7 +3519,7 @@
       <c r="F17" s="15"/>
       <c r="G17" s="103"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>161</v>
       </c>
@@ -3543,7 +3538,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="103"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>165</v>
       </c>
@@ -3562,7 +3557,7 @@
       <c r="F19" s="15"/>
       <c r="G19" s="103"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
@@ -3573,7 +3568,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E20" s="103">
         <v>60</v>
@@ -3581,7 +3576,7 @@
       <c r="F20" s="96"/>
       <c r="G20" s="103"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
@@ -3600,9 +3595,9 @@
       <c r="F21" s="15"/>
       <c r="G21" s="103"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>45</v>
@@ -3611,7 +3606,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="105" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E22" s="103">
         <v>10</v>
@@ -3619,9 +3614,9 @@
       <c r="F22" s="96"/>
       <c r="G22" s="103"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>44</v>
@@ -3630,7 +3625,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="105" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E23" s="103">
         <v>2</v>
@@ -3638,9 +3633,9 @@
       <c r="F23" s="15"/>
       <c r="G23" s="103"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>43</v>
@@ -3649,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="105" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E24" s="103">
         <v>10</v>
@@ -3657,7 +3652,7 @@
       <c r="F24" s="15"/>
       <c r="G24" s="103"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>152</v>
       </c>
@@ -3680,7 +3675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>167</v>
       </c>
@@ -3691,7 +3686,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="105" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E26" s="103">
         <v>73</v>
@@ -3699,18 +3694,18 @@
       <c r="F26" s="15"/>
       <c r="G26" s="103"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="91" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="105" t="s">
         <v>214</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="C27" s="91" t="s">
-        <v>216</v>
-      </c>
-      <c r="D27" s="105" t="s">
-        <v>215</v>
       </c>
       <c r="E27" s="103">
         <v>30</v>
@@ -3718,7 +3713,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="103"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>46</v>
       </c>
@@ -3726,7 +3721,7 @@
         <v>47</v>
       </c>
       <c r="C28" s="91" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D28" s="105" t="s">
         <v>169</v>
@@ -3737,7 +3732,7 @@
       <c r="F28" s="96"/>
       <c r="G28" s="103"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>65</v>
       </c>
@@ -3756,7 +3751,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="103"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>62</v>
       </c>
@@ -3775,7 +3770,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="103"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>56</v>
       </c>
@@ -3794,7 +3789,7 @@
       <c r="F31" s="100"/>
       <c r="G31" s="103"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>51</v>
       </c>
@@ -3805,7 +3800,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="105" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E32" s="103">
         <v>40</v>
@@ -3813,7 +3808,7 @@
       <c r="F32" s="100"/>
       <c r="G32" s="103"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>53</v>
       </c>
@@ -3832,18 +3827,18 @@
       <c r="F33" s="155"/>
       <c r="G33" s="103"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C34" s="91">
         <v>1</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E34" s="103">
         <v>8.5</v>
@@ -3851,18 +3846,18 @@
       <c r="F34" s="15"/>
       <c r="G34" s="103"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B35" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C35" s="91" t="s">
+        <v>219</v>
+      </c>
+      <c r="D35" s="147" t="s">
         <v>221</v>
-      </c>
-      <c r="C35" s="91" t="s">
-        <v>220</v>
-      </c>
-      <c r="D35" s="147" t="s">
-        <v>222</v>
       </c>
       <c r="E35" s="103">
         <v>19</v>
@@ -3870,18 +3865,18 @@
       <c r="F35" s="15"/>
       <c r="G35" s="103"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" s="29" t="s">
         <v>228</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>229</v>
       </c>
       <c r="C36" s="91">
         <v>1</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E36" s="103">
         <v>6</v>
@@ -3889,7 +3884,7 @@
       <c r="F36" s="15"/>
       <c r="G36" s="103"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>48</v>
       </c>
@@ -3908,7 +3903,7 @@
       <c r="F37" s="101"/>
       <c r="G37" s="104"/>
     </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="93" t="s">
         <v>69</v>
       </c>
@@ -3917,12 +3912,12 @@
       <c r="D38" s="94"/>
       <c r="E38" s="95">
         <f>SUBTOTAL(109,Table1[[#All],[Column5]])</f>
-        <v>515.5</v>
+        <v>523.5</v>
       </c>
       <c r="F38" s="64"/>
       <c r="G38" s="64"/>
     </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="124" t="s">
         <v>174</v>
       </c>
@@ -3931,7 +3926,7 @@
       <c r="D39" s="125"/>
       <c r="E39" s="126">
         <f>E4+E38</f>
-        <v>849.5</v>
+        <v>857.5</v>
       </c>
     </row>
   </sheetData>
@@ -3988,101 +3983,101 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="152" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B1" s="152" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C1" s="122"/>
       <c r="D1" s="152" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="B2" s="149" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="149" t="s">
+      <c r="D2" s="142" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="142" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="149" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="149" t="s">
+      <c r="D3" s="150" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="D3" s="150" t="s">
+      <c r="B4" s="142" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="29" t="s">
+      <c r="D4" s="150" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="142" t="s">
-        <v>189</v>
-      </c>
-      <c r="D4" s="150" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="B5" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="142" t="s">
+      <c r="D5" s="150" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="150" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="B6" s="142" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="150" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="B6" s="142" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="150" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="B7" s="150" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="149" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="148" t="s">
         <v>198</v>
       </c>
-      <c r="B7" s="150" t="s">
+      <c r="B8" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="D7" s="149" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="148" t="s">
-        <v>199</v>
-      </c>
-      <c r="B8" s="143" t="s">
-        <v>189</v>
-      </c>
       <c r="D8" s="151" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4096,20 +4091,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -4132,7 +4127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>71</v>
       </c>
@@ -4146,7 +4141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>73</v>
       </c>
@@ -4160,7 +4155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>74</v>
       </c>
@@ -4174,7 +4169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>76</v>
       </c>
@@ -4188,7 +4183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>77</v>
       </c>
@@ -4202,7 +4197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>79</v>
       </c>
@@ -4216,7 +4211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>80</v>
       </c>
@@ -4230,7 +4225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>82</v>
       </c>
@@ -4244,7 +4239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>83</v>
       </c>
@@ -4258,7 +4253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>84</v>
       </c>
@@ -4272,7 +4267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>85</v>
       </c>
@@ -4286,7 +4281,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>123</v>
       </c>
@@ -4300,7 +4295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>86</v>
       </c>
@@ -4314,7 +4309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>88</v>
       </c>
@@ -4328,7 +4323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>89</v>
       </c>
@@ -4342,7 +4337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>90</v>
       </c>
@@ -4356,7 +4351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>91</v>
       </c>
@@ -4370,7 +4365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>92</v>
       </c>
@@ -4384,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>93</v>
       </c>
@@ -4398,7 +4393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>94</v>
       </c>
@@ -4412,7 +4407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>95</v>
       </c>
@@ -4426,7 +4421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>96</v>
       </c>
@@ -4440,7 +4435,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>97</v>
       </c>
@@ -4454,7 +4449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>98</v>
       </c>
@@ -4468,7 +4463,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>100</v>
       </c>
@@ -4485,7 +4480,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>101</v>
       </c>
@@ -4499,7 +4494,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>103</v>
       </c>
@@ -4513,7 +4508,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>104</v>
       </c>
@@ -4527,7 +4522,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>105</v>
       </c>
@@ -4541,7 +4536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>106</v>
       </c>
@@ -4555,7 +4550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
         <v>107</v>
       </c>
@@ -4569,7 +4564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>108</v>
       </c>
@@ -4583,7 +4578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>109</v>
       </c>
@@ -4597,7 +4592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>110</v>
       </c>
@@ -4611,7 +4606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>111</v>
       </c>
@@ -4625,7 +4620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
         <v>112</v>
       </c>
@@ -4639,7 +4634,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="26" t="s">
         <v>113</v>
       </c>
@@ -4649,7 +4644,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>114</v>
       </c>
@@ -4675,14 +4670,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>

</xml_diff>